<commit_message>
making command name lowercase N
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA22F45-CBB5-5744-A066-6F676BF23309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C49AD7E-5F2A-3D45-9EAA-E9A0B982AC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="all_systems" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="142">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="141">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -909,10 +906,10 @@
   <dimension ref="A1:AC47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC48" sqref="AC48"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -940,24 +937,24 @@
   <sheetData>
     <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" s="21"/>
       <c r="J1" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" s="21"/>
       <c r="L1" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
@@ -972,106 +969,106 @@
       <c r="W1" s="21"/>
       <c r="X1" s="12"/>
       <c r="Y1" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z1" s="21"/>
       <c r="AA1" s="22"/>
     </row>
     <row r="2" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="T2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="W2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="W2" s="15" t="s">
+      <c r="X2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="Y2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA2" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -1084,19 +1081,19 @@
         <v>0x80</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="13">
         <v>1</v>
@@ -1141,21 +1138,21 @@
         <v>0</v>
       </c>
       <c r="Z3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA3" s="13">
         <v>0</v>
       </c>
       <c r="AC3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -1168,19 +1165,19 @@
         <v>0x81</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>4</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="13">
         <v>1</v>
@@ -1225,21 +1222,21 @@
         <v>0</v>
       </c>
       <c r="Z4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA4" s="13">
         <v>0</v>
       </c>
       <c r="AC4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -1252,22 +1249,22 @@
         <v>0x82</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="13">
         <v>4</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -1309,21 +1306,21 @@
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA5" s="13">
         <v>0</v>
       </c>
       <c r="AC5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -1336,23 +1333,23 @@
         <v>0x88</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="K6" s="13" t="s">
-        <v>80</v>
-      </c>
       <c r="L6" s="6">
         <v>1</v>
       </c>
@@ -1393,21 +1390,21 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA6" s="13">
         <v>0</v>
       </c>
       <c r="AC6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -1420,22 +1417,22 @@
         <v>0x89</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L7" s="6">
         <v>1</v>
@@ -1477,21 +1474,21 @@
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA7" s="13">
         <v>0</v>
       </c>
       <c r="AC7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -1504,22 +1501,22 @@
         <v>0x8A</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L8" s="6">
         <v>1</v>
@@ -1561,21 +1558,21 @@
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA8" s="13">
         <v>0</v>
       </c>
       <c r="AC8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -1588,22 +1585,22 @@
         <v>0x8B</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L9" s="6">
         <v>1</v>
@@ -1645,21 +1642,21 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA9" s="13">
         <v>0</v>
       </c>
       <c r="AC9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -1672,22 +1669,22 @@
         <v>0x98</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L10" s="6">
         <v>0</v>
@@ -1729,21 +1726,21 @@
         <v>0</v>
       </c>
       <c r="Z10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA10" s="13">
         <v>0</v>
       </c>
       <c r="AC10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -1756,22 +1753,22 @@
         <v>0x9A</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L11" s="6">
         <v>0</v>
@@ -1813,21 +1810,21 @@
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA11" s="13">
         <v>0</v>
       </c>
       <c r="AC11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -1840,22 +1837,22 @@
         <v>0x9C</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L12" s="6">
         <v>0</v>
@@ -1897,21 +1894,21 @@
         <v>0</v>
       </c>
       <c r="Z12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA12" s="13">
         <v>0</v>
       </c>
       <c r="AC12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -1924,19 +1921,19 @@
         <v>0x9D</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K13" s="13">
         <v>8</v>
@@ -1981,21 +1978,21 @@
         <v>0</v>
       </c>
       <c r="Z13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA13" s="13">
         <v>0</v>
       </c>
       <c r="AC13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -2008,19 +2005,19 @@
         <v>0xA1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K14" s="13">
         <v>2</v>
@@ -2065,21 +2062,21 @@
         <v>0</v>
       </c>
       <c r="Z14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA14" s="13">
         <v>0</v>
       </c>
       <c r="AC14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -2092,19 +2089,19 @@
         <v>0xA4</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L15" s="6">
         <v>1</v>
@@ -2146,21 +2143,21 @@
         <v>0</v>
       </c>
       <c r="Z15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA15" s="13">
         <v>0</v>
       </c>
       <c r="AC15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -2173,19 +2170,19 @@
         <v>0xA8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L16" s="6">
         <v>0</v>
@@ -2227,21 +2224,21 @@
         <v>0</v>
       </c>
       <c r="Z16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA16" s="13">
         <v>0</v>
       </c>
       <c r="AC16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -2254,19 +2251,19 @@
         <v>0x92</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L17" s="6">
         <v>0</v>
@@ -2308,21 +2305,21 @@
         <v>0</v>
       </c>
       <c r="Z17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA17" s="13">
         <v>0</v>
       </c>
       <c r="AC17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -2335,19 +2332,19 @@
         <v>0x93</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L18" s="6">
         <v>0</v>
@@ -2389,21 +2386,21 @@
         <v>0</v>
       </c>
       <c r="Z18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA18" s="13">
         <v>0</v>
       </c>
       <c r="AC18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -2416,19 +2413,19 @@
         <v>0xB8</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K19" s="13">
         <v>2</v>
@@ -2473,21 +2470,21 @@
         <v>0</v>
       </c>
       <c r="Z19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA19" s="13">
         <v>0</v>
       </c>
       <c r="AC19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -2500,16 +2497,16 @@
         <v>0xB5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="13">
@@ -2555,21 +2552,21 @@
         <v>0</v>
       </c>
       <c r="Z20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA20" s="13">
         <v>0</v>
       </c>
       <c r="AC20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -2582,16 +2579,16 @@
         <v>0xB6</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="13">
@@ -2637,21 +2634,21 @@
         <v>0</v>
       </c>
       <c r="Z21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA21" s="13">
         <v>0</v>
       </c>
       <c r="AC21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -2664,16 +2661,16 @@
         <v>0xB7</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="13">
@@ -2719,21 +2716,21 @@
         <v>0</v>
       </c>
       <c r="Z22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA22" s="13">
         <v>0</v>
       </c>
       <c r="AC22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -2746,16 +2743,16 @@
         <v>0xB9</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="13">
@@ -2801,13 +2798,13 @@
         <v>0</v>
       </c>
       <c r="Z23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA23" s="13">
         <v>0</v>
       </c>
       <c r="AC23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2839,10 +2836,10 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -2855,22 +2852,22 @@
         <v>0x40</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L25" s="6">
         <v>0</v>
@@ -2912,21 +2909,21 @@
         <v>0</v>
       </c>
       <c r="Z25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA25" s="13">
         <v>0</v>
       </c>
       <c r="AC25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -2939,22 +2936,22 @@
         <v>0x42</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L26" s="6">
         <v>0</v>
@@ -2996,21 +2993,21 @@
         <v>0</v>
       </c>
       <c r="Z26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA26" s="13">
         <v>0</v>
       </c>
       <c r="AC26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -3023,22 +3020,22 @@
         <v>0x44</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L27" s="6">
         <v>1</v>
@@ -3080,21 +3077,21 @@
         <v>0</v>
       </c>
       <c r="Z27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA27" s="13">
         <v>0</v>
       </c>
       <c r="AC27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -3107,22 +3104,22 @@
         <v>0x45</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L28" s="6">
         <v>1</v>
@@ -3164,21 +3161,21 @@
         <v>0</v>
       </c>
       <c r="Z28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA28" s="13">
         <v>0</v>
       </c>
       <c r="AC28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -3191,22 +3188,22 @@
         <v>0x77</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G29">
         <v>2</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L29" s="6">
         <v>1</v>
@@ -3248,21 +3245,21 @@
         <v>0</v>
       </c>
       <c r="Z29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA29" s="13">
         <v>0</v>
       </c>
       <c r="AC29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -3275,22 +3272,22 @@
         <v>0x61</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L30" s="6">
         <v>0</v>
@@ -3332,21 +3329,21 @@
         <v>0</v>
       </c>
       <c r="Z30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA30" s="13">
         <v>0</v>
       </c>
       <c r="AC30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
@@ -3359,14 +3356,14 @@
         <v>0x62</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H31" s="3"/>
       <c r="J31" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L31" s="6">
         <v>0</v>
@@ -3408,21 +3405,21 @@
         <v>0</v>
       </c>
       <c r="Z31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA31" s="13">
         <v>0</v>
       </c>
       <c r="AC31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
@@ -3435,14 +3432,14 @@
         <v>0x63</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H32" s="3"/>
       <c r="J32" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L32" s="6">
         <v>0</v>
@@ -3484,21 +3481,21 @@
         <v>0</v>
       </c>
       <c r="Z32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA32" s="13">
         <v>0</v>
       </c>
       <c r="AC32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C33" s="3">
         <v>0</v>
@@ -3511,14 +3508,14 @@
         <v>0x24</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H33" s="3"/>
       <c r="J33" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L33" s="6">
         <v>1</v>
@@ -3560,21 +3557,21 @@
         <v>0</v>
       </c>
       <c r="Z33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA33" s="13">
         <v>0</v>
       </c>
       <c r="AC33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
@@ -3587,14 +3584,14 @@
         <v>0x25</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H34" s="3"/>
       <c r="J34" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K34" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L34" s="6">
         <v>1</v>
@@ -3636,21 +3633,21 @@
         <v>0</v>
       </c>
       <c r="Z34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA34" s="13">
         <v>0</v>
       </c>
       <c r="AC34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="3">
         <v>0</v>
@@ -3663,23 +3660,23 @@
         <v>0x18</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I35" s="13">
         <f>68*2</f>
         <v>136</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L35" s="6">
         <v>0</v>
@@ -3721,21 +3718,21 @@
         <v>0</v>
       </c>
       <c r="Z35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA35" s="13">
         <v>0</v>
       </c>
       <c r="AC35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
@@ -3748,17 +3745,17 @@
         <v>0x1A</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36" s="3"/>
       <c r="J36" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L36" s="6">
         <v>0</v>
@@ -3800,21 +3797,21 @@
         <v>0</v>
       </c>
       <c r="Z36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA36" s="13">
         <v>0</v>
       </c>
       <c r="AC36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
@@ -3829,10 +3826,10 @@
       <c r="F37" s="3"/>
       <c r="H37" s="3"/>
       <c r="J37" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L37" s="6">
         <v>0</v>
@@ -3874,21 +3871,21 @@
         <v>0</v>
       </c>
       <c r="Z37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA37" s="13">
         <v>0</v>
       </c>
       <c r="AC37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C38" s="3">
         <v>0</v>
@@ -3901,14 +3898,14 @@
         <v>0x1D</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H38" s="3"/>
       <c r="J38" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L38" s="6">
         <v>0</v>
@@ -3950,21 +3947,21 @@
         <v>0</v>
       </c>
       <c r="Z38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA38" s="13">
         <v>0</v>
       </c>
       <c r="AC38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
@@ -3979,10 +3976,10 @@
       <c r="F39" s="3"/>
       <c r="H39" s="3"/>
       <c r="J39" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L39" s="6">
         <v>0</v>
@@ -4024,21 +4021,21 @@
         <v>0</v>
       </c>
       <c r="Z39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA39" s="13">
         <v>0</v>
       </c>
       <c r="AC39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
@@ -4053,10 +4050,10 @@
       <c r="F40" s="3"/>
       <c r="H40" s="3"/>
       <c r="J40" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L40" s="6">
         <v>0</v>
@@ -4098,21 +4095,21 @@
         <v>0</v>
       </c>
       <c r="Z40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA40" s="13">
         <v>0</v>
       </c>
       <c r="AC40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
@@ -4127,10 +4124,10 @@
       <c r="F41" s="3"/>
       <c r="H41" s="3"/>
       <c r="J41" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L41" s="6">
         <v>1</v>
@@ -4172,21 +4169,21 @@
         <v>0</v>
       </c>
       <c r="Z41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA41" s="13">
         <v>0</v>
       </c>
       <c r="AC41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="3">
         <v>0</v>
@@ -4201,10 +4198,10 @@
       <c r="F42" s="3"/>
       <c r="H42" s="3"/>
       <c r="J42" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L42" s="6">
         <v>1</v>
@@ -4246,21 +4243,21 @@
         <v>0</v>
       </c>
       <c r="Z42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA42" s="13">
         <v>0</v>
       </c>
       <c r="AC42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
@@ -4275,10 +4272,10 @@
       <c r="F43" s="3"/>
       <c r="H43" s="3"/>
       <c r="J43" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K43" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L43" s="6">
         <v>1</v>
@@ -4320,21 +4317,21 @@
         <v>0</v>
       </c>
       <c r="Z43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA43" s="13">
         <v>0</v>
       </c>
       <c r="AC43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
@@ -4349,10 +4346,10 @@
       <c r="F44" s="3"/>
       <c r="H44" s="3"/>
       <c r="J44" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L44" s="6">
         <v>1</v>
@@ -4394,21 +4391,21 @@
         <v>0</v>
       </c>
       <c r="Z44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA44" s="13">
         <v>0</v>
       </c>
       <c r="AC44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
@@ -4423,10 +4420,10 @@
       <c r="F45" s="3"/>
       <c r="H45" s="3"/>
       <c r="J45" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L45" s="6">
         <v>1</v>
@@ -4468,21 +4465,21 @@
         <v>0</v>
       </c>
       <c r="Z45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA45" s="13">
         <v>0</v>
       </c>
       <c r="AC45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="3">
         <v>0</v>
@@ -4497,10 +4494,10 @@
       <c r="F46" s="3"/>
       <c r="H46" s="3"/>
       <c r="J46" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L46" s="6">
         <v>1</v>
@@ -4542,21 +4539,21 @@
         <v>0</v>
       </c>
       <c r="Z46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA46" s="13">
         <v>0</v>
       </c>
       <c r="AC46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C47" s="3">
         <v>0</v>
@@ -4571,10 +4568,10 @@
       <c r="F47" s="3"/>
       <c r="H47" s="3"/>
       <c r="J47" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K47" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L47" s="6">
         <v>1</v>
@@ -4616,13 +4613,13 @@
         <v>0</v>
       </c>
       <c r="Z47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA47" s="13">
         <v>0</v>
       </c>
       <c r="AC47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed null tokens from JSON file (for parsability)
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C49AD7E-5F2A-3D45-9EAA-E9A0B982AC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D782FFCB-B7FD-3446-8E19-F65727D8C914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="149">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -457,6 +457,30 @@
   </si>
   <si>
     <t>notify system that power will be cut soon</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>currents</t>
+  </si>
+  <si>
+    <t>voltages</t>
+  </si>
+  <si>
+    <t>outputs</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>thresholds</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>todo</t>
   </si>
 </sst>
 </file>
@@ -906,10 +930,10 @@
   <dimension ref="A1:AC47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,6 +1158,9 @@
       <c r="W3" s="16">
         <v>1</v>
       </c>
+      <c r="X3" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y3" s="18">
         <v>0</v>
       </c>
@@ -1142,6 +1169,9 @@
       </c>
       <c r="AA3" s="13">
         <v>0</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>148</v>
       </c>
       <c r="AC3" t="s">
         <v>101</v>
@@ -1218,6 +1248,9 @@
       <c r="W4" s="16">
         <v>0</v>
       </c>
+      <c r="X4" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y4" s="18">
         <v>0</v>
       </c>
@@ -1226,6 +1259,9 @@
       </c>
       <c r="AA4" s="13">
         <v>0</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>148</v>
       </c>
       <c r="AC4" t="s">
         <v>103</v>
@@ -1302,6 +1338,9 @@
       <c r="W5" s="16">
         <v>0</v>
       </c>
+      <c r="X5" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y5" s="18">
         <v>0</v>
       </c>
@@ -1310,6 +1349,9 @@
       </c>
       <c r="AA5" s="13">
         <v>0</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>148</v>
       </c>
       <c r="AC5" t="s">
         <v>102</v>
@@ -1386,6 +1428,9 @@
       <c r="W6" s="16">
         <v>1</v>
       </c>
+      <c r="X6" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y6" s="18">
         <v>0</v>
       </c>
@@ -1394,6 +1439,9 @@
       </c>
       <c r="AA6" s="13">
         <v>0</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>148</v>
       </c>
       <c r="AC6" t="s">
         <v>104</v>
@@ -1470,6 +1518,9 @@
       <c r="W7" s="16">
         <v>1</v>
       </c>
+      <c r="X7" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y7" s="18">
         <v>0</v>
       </c>
@@ -1478,6 +1529,9 @@
       </c>
       <c r="AA7" s="13">
         <v>0</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>148</v>
       </c>
       <c r="AC7" t="s">
         <v>105</v>
@@ -1554,6 +1608,9 @@
       <c r="W8" s="16">
         <v>1</v>
       </c>
+      <c r="X8" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y8" s="18">
         <v>0</v>
       </c>
@@ -1562,6 +1619,9 @@
       </c>
       <c r="AA8" s="13">
         <v>0</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>148</v>
       </c>
       <c r="AC8" t="s">
         <v>106</v>
@@ -1638,6 +1698,9 @@
       <c r="W9" s="16">
         <v>1</v>
       </c>
+      <c r="X9" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y9" s="18">
         <v>0</v>
       </c>
@@ -1646,6 +1709,9 @@
       </c>
       <c r="AA9" s="13">
         <v>0</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>148</v>
       </c>
       <c r="AC9" t="s">
         <v>107</v>
@@ -1722,6 +1788,9 @@
       <c r="W10" s="16">
         <v>0</v>
       </c>
+      <c r="X10" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y10" s="18">
         <v>0</v>
       </c>
@@ -1730,6 +1799,9 @@
       </c>
       <c r="AA10" s="13">
         <v>0</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>148</v>
       </c>
       <c r="AC10" t="s">
         <v>108</v>
@@ -1806,6 +1878,9 @@
       <c r="W11" s="16">
         <v>0</v>
       </c>
+      <c r="X11" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y11" s="18">
         <v>0</v>
       </c>
@@ -1814,6 +1889,9 @@
       </c>
       <c r="AA11" s="13">
         <v>0</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>148</v>
       </c>
       <c r="AC11" t="s">
         <v>109</v>
@@ -1890,6 +1968,9 @@
       <c r="W12" s="16">
         <v>0</v>
       </c>
+      <c r="X12" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y12" s="18">
         <v>0</v>
       </c>
@@ -1898,6 +1979,9 @@
       </c>
       <c r="AA12" s="13">
         <v>0</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>148</v>
       </c>
       <c r="AC12" t="s">
         <v>110</v>
@@ -1974,6 +2058,9 @@
       <c r="W13" s="16">
         <v>0</v>
       </c>
+      <c r="X13" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y13" s="18">
         <v>0</v>
       </c>
@@ -1982,6 +2069,9 @@
       </c>
       <c r="AA13" s="13">
         <v>0</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>148</v>
       </c>
       <c r="AC13" t="s">
         <v>111</v>
@@ -2058,6 +2148,9 @@
       <c r="W14" s="16">
         <v>1</v>
       </c>
+      <c r="X14" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y14" s="18">
         <v>0</v>
       </c>
@@ -2066,6 +2159,9 @@
       </c>
       <c r="AA14" s="13">
         <v>0</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>148</v>
       </c>
       <c r="AC14" t="s">
         <v>112</v>
@@ -2103,6 +2199,9 @@
       <c r="J15" s="3" t="s">
         <v>85</v>
       </c>
+      <c r="K15" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="L15" s="6">
         <v>1</v>
       </c>
@@ -2138,6 +2237,9 @@
       </c>
       <c r="W15" s="16">
         <v>1</v>
+      </c>
+      <c r="X15" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y15" s="18">
         <v>0</v>
@@ -2147,6 +2249,9 @@
       </c>
       <c r="AA15" s="13">
         <v>0</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>148</v>
       </c>
       <c r="AC15" t="s">
         <v>113</v>
@@ -2184,6 +2289,9 @@
       <c r="J16" s="3" t="s">
         <v>96</v>
       </c>
+      <c r="K16" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="L16" s="6">
         <v>0</v>
       </c>
@@ -2219,6 +2327,9 @@
       </c>
       <c r="W16" s="16">
         <v>1</v>
+      </c>
+      <c r="X16" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y16" s="18">
         <v>0</v>
@@ -2228,6 +2339,9 @@
       </c>
       <c r="AA16" s="13">
         <v>0</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>148</v>
       </c>
       <c r="AC16" t="s">
         <v>100</v>
@@ -2265,6 +2379,9 @@
       <c r="J17" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="K17" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="L17" s="6">
         <v>0</v>
       </c>
@@ -2300,6 +2417,9 @@
       </c>
       <c r="W17" s="16">
         <v>0</v>
+      </c>
+      <c r="X17" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y17" s="18">
         <v>0</v>
@@ -2309,6 +2429,9 @@
       </c>
       <c r="AA17" s="13">
         <v>0</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>148</v>
       </c>
       <c r="AC17" t="s">
         <v>114</v>
@@ -2346,6 +2469,9 @@
       <c r="J18" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="K18" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="L18" s="6">
         <v>0</v>
       </c>
@@ -2381,6 +2507,9 @@
       </c>
       <c r="W18" s="16">
         <v>0</v>
+      </c>
+      <c r="X18" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y18" s="18">
         <v>0</v>
@@ -2390,6 +2519,9 @@
       </c>
       <c r="AA18" s="13">
         <v>0</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>148</v>
       </c>
       <c r="AC18" t="s">
         <v>115</v>
@@ -2466,6 +2598,9 @@
       <c r="W19" s="16">
         <v>0</v>
       </c>
+      <c r="X19" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y19" s="18">
         <v>0</v>
       </c>
@@ -2474,6 +2609,9 @@
       </c>
       <c r="AA19" s="13">
         <v>0</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>148</v>
       </c>
       <c r="AC19" t="s">
         <v>99</v>
@@ -2508,7 +2646,9 @@
       <c r="I20" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="3"/>
+      <c r="J20" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="K20" s="13">
         <v>1</v>
       </c>
@@ -2547,6 +2687,9 @@
       </c>
       <c r="W20" s="16">
         <v>0</v>
+      </c>
+      <c r="X20" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y20" s="18">
         <v>0</v>
@@ -2556,6 +2699,9 @@
       </c>
       <c r="AA20" s="13">
         <v>0</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>148</v>
       </c>
       <c r="AC20" t="s">
         <v>116</v>
@@ -2590,7 +2736,9 @@
       <c r="I21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="3"/>
+      <c r="J21" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="K21" s="13">
         <v>1</v>
       </c>
@@ -2629,6 +2777,9 @@
       </c>
       <c r="W21" s="16">
         <v>0</v>
+      </c>
+      <c r="X21" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y21" s="18">
         <v>0</v>
@@ -2638,6 +2789,9 @@
       </c>
       <c r="AA21" s="13">
         <v>0</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>148</v>
       </c>
       <c r="AC21" t="s">
         <v>117</v>
@@ -2672,7 +2826,9 @@
       <c r="I22" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="3"/>
+      <c r="J22" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="K22" s="13">
         <v>2</v>
       </c>
@@ -2712,6 +2868,9 @@
       <c r="W22" s="16">
         <v>0</v>
       </c>
+      <c r="X22" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y22" s="18">
         <v>0</v>
       </c>
@@ -2720,6 +2879,9 @@
       </c>
       <c r="AA22" s="13">
         <v>0</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>148</v>
       </c>
       <c r="AC22" t="s">
         <v>118</v>
@@ -2754,7 +2916,9 @@
       <c r="I23" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="3"/>
+      <c r="J23" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="K23" s="13">
         <v>1</v>
       </c>
@@ -2793,6 +2957,9 @@
       </c>
       <c r="W23" s="16">
         <v>0</v>
+      </c>
+      <c r="X23" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y23" s="18">
         <v>0</v>
@@ -2802,6 +2969,9 @@
       </c>
       <c r="AA23" s="13">
         <v>0</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>148</v>
       </c>
       <c r="AC23" t="s">
         <v>119</v>
@@ -2905,6 +3075,9 @@
       <c r="W25" s="16">
         <v>0</v>
       </c>
+      <c r="X25" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y25" s="18">
         <v>0</v>
       </c>
@@ -2913,6 +3086,9 @@
       </c>
       <c r="AA25" s="13">
         <v>0</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>148</v>
       </c>
       <c r="AC25" t="s">
         <v>120</v>
@@ -2989,6 +3165,9 @@
       <c r="W26" s="16">
         <v>0</v>
       </c>
+      <c r="X26" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y26" s="18">
         <v>0</v>
       </c>
@@ -2997,6 +3176,9 @@
       </c>
       <c r="AA26" s="13">
         <v>0</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>148</v>
       </c>
       <c r="AC26" t="s">
         <v>121</v>
@@ -3073,6 +3255,9 @@
       <c r="W27" s="16">
         <v>0</v>
       </c>
+      <c r="X27" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y27" s="18">
         <v>0</v>
       </c>
@@ -3081,6 +3266,9 @@
       </c>
       <c r="AA27" s="13">
         <v>0</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>148</v>
       </c>
       <c r="AC27" t="s">
         <v>77</v>
@@ -3157,6 +3345,9 @@
       <c r="W28" s="16">
         <v>0</v>
       </c>
+      <c r="X28" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y28" s="18">
         <v>0</v>
       </c>
@@ -3165,6 +3356,9 @@
       </c>
       <c r="AA28" s="13">
         <v>0</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>148</v>
       </c>
       <c r="AC28" t="s">
         <v>77</v>
@@ -3241,6 +3435,9 @@
       <c r="W29" s="16">
         <v>0</v>
       </c>
+      <c r="X29" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y29" s="18">
         <v>0</v>
       </c>
@@ -3249,6 +3446,9 @@
       </c>
       <c r="AA29" s="13">
         <v>0</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>148</v>
       </c>
       <c r="AC29" t="s">
         <v>122</v>
@@ -3325,6 +3525,9 @@
       <c r="W30" s="16">
         <v>1</v>
       </c>
+      <c r="X30" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y30" s="18">
         <v>0</v>
       </c>
@@ -3333,6 +3536,9 @@
       </c>
       <c r="AA30" s="13">
         <v>0</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>148</v>
       </c>
       <c r="AC30" t="s">
         <v>123</v>
@@ -3358,7 +3564,15 @@
       <c r="F31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="3"/>
+      <c r="G31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J31" s="3" t="s">
         <v>17</v>
       </c>
@@ -3400,6 +3614,9 @@
       </c>
       <c r="W31" s="16">
         <v>1</v>
+      </c>
+      <c r="X31" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y31" s="18">
         <v>0</v>
@@ -3409,6 +3626,9 @@
       </c>
       <c r="AA31" s="13">
         <v>0</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>148</v>
       </c>
       <c r="AC31" t="s">
         <v>124</v>
@@ -3434,7 +3654,15 @@
       <c r="F32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="3"/>
+      <c r="G32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J32" s="3" t="s">
         <v>17</v>
       </c>
@@ -3476,6 +3704,9 @@
       </c>
       <c r="W32" s="16">
         <v>1</v>
+      </c>
+      <c r="X32" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y32" s="18">
         <v>0</v>
@@ -3485,6 +3716,9 @@
       </c>
       <c r="AA32" s="13">
         <v>0</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>148</v>
       </c>
       <c r="AC32" t="s">
         <v>125</v>
@@ -3510,7 +3744,15 @@
       <c r="F33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="3"/>
+      <c r="G33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J33" s="3" t="s">
         <v>17</v>
       </c>
@@ -3552,6 +3794,9 @@
       </c>
       <c r="W33" s="16">
         <v>1</v>
+      </c>
+      <c r="X33" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y33" s="18">
         <v>0</v>
@@ -3561,6 +3806,9 @@
       </c>
       <c r="AA33" s="13">
         <v>0</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>148</v>
       </c>
       <c r="AC33" t="s">
         <v>126</v>
@@ -3586,7 +3834,15 @@
       <c r="F34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="3"/>
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J34" s="3" t="s">
         <v>17</v>
       </c>
@@ -3628,6 +3884,9 @@
       </c>
       <c r="W34" s="16">
         <v>1</v>
+      </c>
+      <c r="X34" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y34" s="18">
         <v>0</v>
@@ -3637,6 +3896,9 @@
       </c>
       <c r="AA34" s="13">
         <v>0</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>148</v>
       </c>
       <c r="AC34" t="s">
         <v>127</v>
@@ -3714,6 +3976,9 @@
       <c r="W35" s="16">
         <v>0</v>
       </c>
+      <c r="X35" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="Y35" s="18">
         <v>0</v>
       </c>
@@ -3722,6 +3987,9 @@
       </c>
       <c r="AA35" s="13">
         <v>0</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>148</v>
       </c>
       <c r="AC35" t="s">
         <v>128</v>
@@ -3750,7 +4018,12 @@
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="H36" s="3"/>
+      <c r="H36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J36" s="3" t="s">
         <v>17</v>
       </c>
@@ -3792,6 +4065,9 @@
       </c>
       <c r="W36" s="16">
         <v>0</v>
+      </c>
+      <c r="X36" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y36" s="18">
         <v>0</v>
@@ -3801,6 +4077,9 @@
       </c>
       <c r="AA36" s="13">
         <v>0</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>148</v>
       </c>
       <c r="AC36" t="s">
         <v>129</v>
@@ -3823,8 +4102,18 @@
         <f t="shared" si="1"/>
         <v>0x1C</v>
       </c>
-      <c r="F37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G37" t="s">
+        <v>141</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J37" s="3" t="s">
         <v>17</v>
       </c>
@@ -3866,6 +4155,9 @@
       </c>
       <c r="W37" s="16">
         <v>0</v>
+      </c>
+      <c r="X37" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y37" s="18">
         <v>0</v>
@@ -3875,6 +4167,9 @@
       </c>
       <c r="AA37" s="13">
         <v>0</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>148</v>
       </c>
       <c r="AC37" t="s">
         <v>130</v>
@@ -3900,7 +4195,15 @@
       <c r="F38" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H38" s="3"/>
+      <c r="G38" t="s">
+        <v>141</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J38" s="3" t="s">
         <v>17</v>
       </c>
@@ -3942,6 +4245,9 @@
       </c>
       <c r="W38" s="16">
         <v>0</v>
+      </c>
+      <c r="X38" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y38" s="18">
         <v>0</v>
@@ -3951,6 +4257,9 @@
       </c>
       <c r="AA38" s="13">
         <v>0</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>148</v>
       </c>
       <c r="AC38" t="s">
         <v>131</v>
@@ -3973,8 +4282,18 @@
         <f t="shared" si="1"/>
         <v>0x12</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G39" t="s">
+        <v>141</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J39" s="3" t="s">
         <v>17</v>
       </c>
@@ -4016,6 +4335,9 @@
       </c>
       <c r="W39" s="16">
         <v>0</v>
+      </c>
+      <c r="X39" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y39" s="18">
         <v>0</v>
@@ -4025,6 +4347,9 @@
       </c>
       <c r="AA39" s="13">
         <v>0</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>148</v>
       </c>
       <c r="AC39" t="s">
         <v>132</v>
@@ -4047,8 +4372,18 @@
         <f t="shared" si="1"/>
         <v>0x13</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G40" t="s">
+        <v>141</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J40" s="3" t="s">
         <v>17</v>
       </c>
@@ -4090,6 +4425,9 @@
       </c>
       <c r="W40" s="16">
         <v>0</v>
+      </c>
+      <c r="X40" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y40" s="18">
         <v>0</v>
@@ -4099,6 +4437,9 @@
       </c>
       <c r="AA40" s="13">
         <v>0</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>148</v>
       </c>
       <c r="AC40" t="s">
         <v>133</v>
@@ -4121,8 +4462,18 @@
         <f t="shared" si="1"/>
         <v>0x39</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="F41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J41" s="3" t="s">
         <v>17</v>
       </c>
@@ -4164,6 +4515,9 @@
       </c>
       <c r="W41" s="16">
         <v>0</v>
+      </c>
+      <c r="X41" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y41" s="18">
         <v>0</v>
@@ -4173,6 +4527,9 @@
       </c>
       <c r="AA41" s="13">
         <v>0</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>148</v>
       </c>
       <c r="AC41" t="s">
         <v>134</v>
@@ -4195,8 +4552,18 @@
         <f t="shared" si="1"/>
         <v>0x70</v>
       </c>
-      <c r="F42" s="3"/>
-      <c r="H42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J42" s="3" t="s">
         <v>17</v>
       </c>
@@ -4238,6 +4605,9 @@
       </c>
       <c r="W42" s="16">
         <v>1</v>
+      </c>
+      <c r="X42" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y42" s="18">
         <v>0</v>
@@ -4247,6 +4617,9 @@
       </c>
       <c r="AA42" s="13">
         <v>0</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>148</v>
       </c>
       <c r="AC42" t="s">
         <v>135</v>
@@ -4269,8 +4642,18 @@
         <f t="shared" si="1"/>
         <v>0x71</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="H43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J43" s="3" t="s">
         <v>17</v>
       </c>
@@ -4312,6 +4695,9 @@
       </c>
       <c r="W43" s="16">
         <v>1</v>
+      </c>
+      <c r="X43" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y43" s="18">
         <v>0</v>
@@ -4321,6 +4707,9 @@
       </c>
       <c r="AA43" s="13">
         <v>0</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>148</v>
       </c>
       <c r="AC43" t="s">
         <v>136</v>
@@ -4343,8 +4732,18 @@
         <f t="shared" si="1"/>
         <v>0x72</v>
       </c>
-      <c r="F44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J44" s="3" t="s">
         <v>17</v>
       </c>
@@ -4386,6 +4785,9 @@
       </c>
       <c r="W44" s="16">
         <v>1</v>
+      </c>
+      <c r="X44" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y44" s="18">
         <v>0</v>
@@ -4395,6 +4797,9 @@
       </c>
       <c r="AA44" s="13">
         <v>0</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>148</v>
       </c>
       <c r="AC44" t="s">
         <v>137</v>
@@ -4417,8 +4822,18 @@
         <f t="shared" si="1"/>
         <v>0x73</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="H45" s="3"/>
+      <c r="F45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J45" s="3" t="s">
         <v>17</v>
       </c>
@@ -4460,6 +4875,9 @@
       </c>
       <c r="W45" s="16">
         <v>1</v>
+      </c>
+      <c r="X45" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y45" s="18">
         <v>0</v>
@@ -4469,6 +4887,9 @@
       </c>
       <c r="AA45" s="13">
         <v>0</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>148</v>
       </c>
       <c r="AC45" t="s">
         <v>138</v>
@@ -4491,8 +4912,18 @@
         <f t="shared" ref="E46:E47" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C46,7) + BIN2DEC($D46)))</f>
         <v>0x74</v>
       </c>
-      <c r="F46" s="3"/>
-      <c r="H46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J46" s="3" t="s">
         <v>17</v>
       </c>
@@ -4534,6 +4965,9 @@
       </c>
       <c r="W46" s="16">
         <v>1</v>
+      </c>
+      <c r="X46" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y46" s="18">
         <v>0</v>
@@ -4543,6 +4977,9 @@
       </c>
       <c r="AA46" s="13">
         <v>0</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>148</v>
       </c>
       <c r="AC46" t="s">
         <v>139</v>
@@ -4565,8 +5002,18 @@
         <f t="shared" si="2"/>
         <v>0x78</v>
       </c>
-      <c r="F47" s="3"/>
-      <c r="H47" s="3"/>
+      <c r="F47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="J47" s="3" t="s">
         <v>17</v>
       </c>
@@ -4608,6 +5055,9 @@
       </c>
       <c r="W47" s="16">
         <v>1</v>
+      </c>
+      <c r="X47" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="Y47" s="18">
         <v>0</v>
@@ -4617,6 +5067,9 @@
       </c>
       <c r="AA47" s="13">
         <v>0</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>148</v>
       </c>
       <c r="AC47" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
adding basic cdte commands
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D782FFCB-B7FD-3446-8E19-F65727D8C914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F39F2B-2968-2F4E-B6E0-EF1F60DD085E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="168">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -481,6 +481,63 @@
   </si>
   <si>
     <t>todo</t>
+  </si>
+  <si>
+    <t>set_de_idle</t>
+  </si>
+  <si>
+    <t>set_de_standby</t>
+  </si>
+  <si>
+    <t>set_de_setup_done</t>
+  </si>
+  <si>
+    <t>set_de_observe</t>
+  </si>
+  <si>
+    <t>set_de_end_op</t>
+  </si>
+  <si>
+    <t>0x022b0000</t>
+  </si>
+  <si>
+    <t>set_can_idle</t>
+  </si>
+  <si>
+    <t>set_can_copy_data</t>
+  </si>
+  <si>
+    <t>set_can_end</t>
+  </si>
+  <si>
+    <t>set_can_run</t>
+  </si>
+  <si>
+    <t>0x3c3c0100010101013c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100020202023c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100030303033c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100040404043c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100050505053c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100060606063c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100000000003c3c3c</t>
+  </si>
+  <si>
+    <t>set the DE mode</t>
+  </si>
+  <si>
+    <t>set the canister mode</t>
   </si>
 </sst>
 </file>
@@ -492,7 +549,7 @@
     <numFmt numFmtId="165" formatCode="00\ 0000\ 00"/>
     <numFmt numFmtId="166" formatCode="0000\ ####"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -519,6 +576,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -565,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -600,10 +676,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -927,16 +1009,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC47"/>
+  <dimension ref="A1:AC56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -952,53 +1034,53 @@
     <col min="12" max="22" width="9.33203125" customWidth="1"/>
     <col min="23" max="23" width="9.33203125" style="13" customWidth="1"/>
     <col min="24" max="24" width="10.83203125" style="13"/>
-    <col min="25" max="25" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.5" style="21" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19.1640625" customWidth="1"/>
     <col min="29" max="29" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="21" t="s">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21" t="s">
+      <c r="K1" s="27"/>
+      <c r="L1" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
       <c r="X1" s="12"/>
-      <c r="Y1" s="20" t="s">
+      <c r="Y1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="22"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="28"/>
     </row>
-    <row r="2" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1087,11 +1169,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C3" s="3">
@@ -1161,13 +1243,13 @@
       <c r="X3" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y3" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="Y3" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA3" s="13">
+      <c r="AA3" s="23">
         <v>0</v>
       </c>
       <c r="AB3" t="s">
@@ -1177,11 +1259,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C4" s="3">
@@ -1251,13 +1333,13 @@
       <c r="X4" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y4" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="Y4" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA4" s="13">
+      <c r="AA4" s="23">
         <v>0</v>
       </c>
       <c r="AB4" t="s">
@@ -1267,11 +1349,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C5" s="3">
@@ -1341,13 +1423,13 @@
       <c r="X5" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y5" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="s">
+      <c r="Y5" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA5" s="13">
+      <c r="AA5" s="23">
         <v>0</v>
       </c>
       <c r="AB5" t="s">
@@ -1357,11 +1439,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C6" s="3">
@@ -1431,13 +1513,13 @@
       <c r="X6" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y6" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="Y6" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA6" s="13">
+      <c r="AA6" s="23">
         <v>0</v>
       </c>
       <c r="AB6" t="s">
@@ -1447,11 +1529,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C7" s="3">
@@ -1521,13 +1603,13 @@
       <c r="X7" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y7" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z7" t="s">
+      <c r="Y7" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA7" s="13">
+      <c r="AA7" s="23">
         <v>0</v>
       </c>
       <c r="AB7" t="s">
@@ -1537,11 +1619,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C8" s="3">
@@ -1611,13 +1693,13 @@
       <c r="X8" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y8" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z8" t="s">
+      <c r="Y8" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA8" s="13">
+      <c r="AA8" s="23">
         <v>0</v>
       </c>
       <c r="AB8" t="s">
@@ -1627,11 +1709,11 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C9" s="3">
@@ -1701,13 +1783,13 @@
       <c r="X9" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y9" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z9" t="s">
+      <c r="Y9" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA9" s="13">
+      <c r="AA9" s="23">
         <v>0</v>
       </c>
       <c r="AB9" t="s">
@@ -1717,11 +1799,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C10" s="3">
@@ -1791,13 +1873,13 @@
       <c r="X10" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y10" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z10" t="s">
+      <c r="Y10" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA10" s="13">
+      <c r="AA10" s="23">
         <v>0</v>
       </c>
       <c r="AB10" t="s">
@@ -1807,11 +1889,11 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C11" s="3">
@@ -1881,13 +1963,13 @@
       <c r="X11" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y11" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="s">
+      <c r="Y11" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA11" s="13">
+      <c r="AA11" s="23">
         <v>0</v>
       </c>
       <c r="AB11" t="s">
@@ -1897,11 +1979,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C12" s="3">
@@ -1971,13 +2053,13 @@
       <c r="X12" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y12" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z12" t="s">
+      <c r="Y12" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA12" s="13">
+      <c r="AA12" s="23">
         <v>0</v>
       </c>
       <c r="AB12" t="s">
@@ -1987,11 +2069,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C13" s="3">
@@ -2061,13 +2143,13 @@
       <c r="X13" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y13" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z13" t="s">
+      <c r="Y13" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA13" s="13">
+      <c r="AA13" s="23">
         <v>0</v>
       </c>
       <c r="AB13" t="s">
@@ -2077,11 +2159,11 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C14" s="3">
@@ -2151,13 +2233,13 @@
       <c r="X14" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y14" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z14" t="s">
+      <c r="Y14" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA14" s="13">
+      <c r="AA14" s="23">
         <v>0</v>
       </c>
       <c r="AB14" t="s">
@@ -2167,11 +2249,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="3">
@@ -2241,13 +2323,13 @@
       <c r="X15" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y15" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z15" t="s">
+      <c r="Y15" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA15" s="13">
+      <c r="AA15" s="23">
         <v>0</v>
       </c>
       <c r="AB15" t="s">
@@ -2257,11 +2339,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C16" s="3">
@@ -2331,13 +2413,13 @@
       <c r="X16" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y16" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="s">
+      <c r="Y16" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA16" s="13">
+      <c r="AA16" s="23">
         <v>0</v>
       </c>
       <c r="AB16" t="s">
@@ -2347,11 +2429,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C17" s="3">
@@ -2421,13 +2503,13 @@
       <c r="X17" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y17" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z17" t="s">
+      <c r="Y17" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA17" s="13">
+      <c r="AA17" s="23">
         <v>0</v>
       </c>
       <c r="AB17" t="s">
@@ -2437,11 +2519,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C18" s="3">
@@ -2511,13 +2593,13 @@
       <c r="X18" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y18" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="s">
+      <c r="Y18" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA18" s="13">
+      <c r="AA18" s="23">
         <v>0</v>
       </c>
       <c r="AB18" t="s">
@@ -2527,11 +2609,11 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C19" s="3">
@@ -2601,13 +2683,13 @@
       <c r="X19" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y19" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z19" t="s">
+      <c r="Y19" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA19" s="13">
+      <c r="AA19" s="23">
         <v>0</v>
       </c>
       <c r="AB19" t="s">
@@ -2617,11 +2699,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C20" s="3">
@@ -2691,13 +2773,13 @@
       <c r="X20" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y20" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z20" t="s">
+      <c r="Y20" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA20" s="13">
+      <c r="AA20" s="23">
         <v>0</v>
       </c>
       <c r="AB20" t="s">
@@ -2707,11 +2789,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C21" s="3">
@@ -2781,13 +2863,13 @@
       <c r="X21" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y21" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z21" t="s">
+      <c r="Y21" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA21" s="13">
+      <c r="AA21" s="23">
         <v>0</v>
       </c>
       <c r="AB21" t="s">
@@ -2797,11 +2879,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C22" s="3">
@@ -2871,13 +2953,13 @@
       <c r="X22" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y22" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z22" t="s">
+      <c r="Y22" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA22" s="13">
+      <c r="AA22" s="23">
         <v>0</v>
       </c>
       <c r="AB22" t="s">
@@ -2887,11 +2969,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C23" s="3">
@@ -2961,13 +3043,13 @@
       <c r="X23" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y23" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z23" t="s">
+      <c r="Y23" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA23" s="13">
+      <c r="AA23" s="23">
         <v>0</v>
       </c>
       <c r="AB23" t="s">
@@ -3001,14 +3083,15 @@
       <c r="V24" s="9"/>
       <c r="W24" s="17"/>
       <c r="X24" s="14"/>
-      <c r="Y24" s="14"/>
-      <c r="AA24" s="14"/>
+      <c r="Y24" s="24"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="24"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C25" s="3">
@@ -3018,7 +3101,7 @@
         <v>1000000</v>
       </c>
       <c r="E25" s="3" t="str">
-        <f t="shared" ref="E25:E45" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C25,7) + BIN2DEC($D25)))</f>
+        <f t="shared" ref="E25:E54" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C25,7) + BIN2DEC($D25)))</f>
         <v>0x40</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -3078,13 +3161,13 @@
       <c r="X25" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y25" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z25" t="s">
+      <c r="Y25" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA25" s="13">
+      <c r="AA25" s="23">
         <v>0</v>
       </c>
       <c r="AB25" t="s">
@@ -3094,11 +3177,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C26" s="3">
@@ -3168,13 +3251,13 @@
       <c r="X26" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y26" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z26" t="s">
+      <c r="Y26" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA26" s="13">
+      <c r="AA26" s="23">
         <v>0</v>
       </c>
       <c r="AB26" t="s">
@@ -3184,11 +3267,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C27" s="3">
@@ -3258,13 +3341,13 @@
       <c r="X27" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y27" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z27" t="s">
+      <c r="Y27" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA27" s="13">
+      <c r="AA27" s="23">
         <v>0</v>
       </c>
       <c r="AB27" t="s">
@@ -3274,11 +3357,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C28" s="3">
@@ -3348,13 +3431,13 @@
       <c r="X28" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y28" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z28" t="s">
+      <c r="Y28" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA28" s="13">
+      <c r="AA28" s="23">
         <v>0</v>
       </c>
       <c r="AB28" t="s">
@@ -3364,11 +3447,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C29" s="3">
@@ -3438,13 +3521,13 @@
       <c r="X29" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y29" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z29" t="s">
+      <c r="Y29" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA29" s="13">
+      <c r="AA29" s="23">
         <v>0</v>
       </c>
       <c r="AB29" t="s">
@@ -3454,11 +3537,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C30" s="3">
@@ -3528,13 +3611,13 @@
       <c r="X30" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y30" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z30" t="s">
+      <c r="Y30" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA30" s="13">
+      <c r="AA30" s="23">
         <v>0</v>
       </c>
       <c r="AB30" t="s">
@@ -3544,11 +3627,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C31" s="3">
@@ -3618,13 +3701,13 @@
       <c r="X31" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y31" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z31" t="s">
+      <c r="Y31" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA31" s="13">
+      <c r="AA31" s="23">
         <v>0</v>
       </c>
       <c r="AB31" t="s">
@@ -3634,11 +3717,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C32" s="3">
@@ -3708,13 +3791,13 @@
       <c r="X32" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y32" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z32" t="s">
+      <c r="Y32" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA32" s="13">
+      <c r="AA32" s="23">
         <v>0</v>
       </c>
       <c r="AB32" t="s">
@@ -3724,11 +3807,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C33" s="3">
@@ -3798,13 +3881,13 @@
       <c r="X33" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y33" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z33" t="s">
+      <c r="Y33" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA33" s="13">
+      <c r="AA33" s="23">
         <v>0</v>
       </c>
       <c r="AB33" t="s">
@@ -3814,11 +3897,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C34" s="3">
@@ -3888,13 +3971,13 @@
       <c r="X34" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y34" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z34" t="s">
+      <c r="Y34" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA34" s="13">
+      <c r="AA34" s="23">
         <v>0</v>
       </c>
       <c r="AB34" t="s">
@@ -3904,11 +3987,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C35" s="3">
@@ -3918,7 +4001,7 @@
         <v>11000</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C35,7) + BIN2DEC($D35)))</f>
         <v>0x18</v>
       </c>
       <c r="F35" s="3" t="s">
@@ -3979,14 +4062,14 @@
       <c r="X35" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y35" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z35" t="s">
+      <c r="Y35" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA35" s="13">
-        <v>0</v>
+      <c r="AA35" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="AB35" t="s">
         <v>148</v>
@@ -3995,28 +4078,28 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B36" s="19" t="s">
+    <row r="36" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
       </c>
       <c r="D36" s="10">
-        <v>11010</v>
+        <v>11111</v>
       </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1A</v>
+        <v>0x1F</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>17</v>
@@ -4024,7 +4107,7 @@
       <c r="I36" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="J36" t="s">
         <v>17</v>
       </c>
       <c r="K36" s="13" t="s">
@@ -4043,16 +4126,16 @@
         <v>0</v>
       </c>
       <c r="P36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T36" s="6">
         <v>1</v>
@@ -4069,44 +4152,44 @@
       <c r="X36" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y36" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z36" t="s">
+      <c r="Y36" s="22">
+        <v>1100100</v>
+      </c>
+      <c r="Z36" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA36" s="13">
-        <v>0</v>
+      <c r="AA36" s="23" t="s">
+        <v>160</v>
       </c>
       <c r="AB36" t="s">
         <v>148</v>
       </c>
       <c r="AC36" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="19" t="s">
+    <row r="37" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>11100</v>
+        <v>10000</v>
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1C</v>
+        <v>0x10</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G37" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>17</v>
@@ -4114,7 +4197,7 @@
       <c r="I37" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="J37" t="s">
         <v>17</v>
       </c>
       <c r="K37" s="13" t="s">
@@ -4133,16 +4216,16 @@
         <v>0</v>
       </c>
       <c r="P37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T37" s="6">
         <v>1</v>
@@ -4159,44 +4242,44 @@
       <c r="X37" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y37" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z37" t="s">
+      <c r="Y37" s="22">
+        <v>1100100</v>
+      </c>
+      <c r="Z37" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA37" s="13">
-        <v>0</v>
+      <c r="AA37" s="25" t="s">
+        <v>161</v>
       </c>
       <c r="AB37" t="s">
         <v>148</v>
       </c>
       <c r="AC37" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="19" t="s">
+    <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C38" s="3">
         <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>11101</v>
+        <v>10001</v>
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1D</v>
+        <v>0x11</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="G38" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>17</v>
@@ -4204,7 +4287,7 @@
       <c r="I38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J38" t="s">
         <v>17</v>
       </c>
       <c r="K38" s="13" t="s">
@@ -4223,16 +4306,16 @@
         <v>0</v>
       </c>
       <c r="P38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T38" s="6">
         <v>1</v>
@@ -4249,28 +4332,28 @@
       <c r="X38" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y38" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z38" t="s">
+      <c r="Y38" s="22">
+        <v>1100100</v>
+      </c>
+      <c r="Z38" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA38" s="13">
-        <v>0</v>
+      <c r="AA38" s="25" t="s">
+        <v>162</v>
       </c>
       <c r="AB38" t="s">
         <v>148</v>
       </c>
       <c r="AC38" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>98</v>
+    <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
@@ -4283,10 +4366,10 @@
         <v>0x12</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="G39" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>17</v>
@@ -4294,7 +4377,7 @@
       <c r="I39" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="J39" t="s">
         <v>17</v>
       </c>
       <c r="K39" s="13" t="s">
@@ -4325,13 +4408,13 @@
         <v>0</v>
       </c>
       <c r="T39" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U39" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V39" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W39" s="16">
         <v>0</v>
@@ -4339,28 +4422,28 @@
       <c r="X39" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y39" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z39" t="s">
+      <c r="Y39" s="22">
+        <v>1100100</v>
+      </c>
+      <c r="Z39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA39" s="13">
-        <v>0</v>
+      <c r="AA39" s="25" t="s">
+        <v>163</v>
       </c>
       <c r="AB39" t="s">
         <v>148</v>
       </c>
       <c r="AC39" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>98</v>
+    <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
@@ -4373,10 +4456,10 @@
         <v>0x13</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="G40" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>17</v>
@@ -4384,7 +4467,7 @@
       <c r="I40" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J40" s="3" t="s">
+      <c r="J40" t="s">
         <v>17</v>
       </c>
       <c r="K40" s="13" t="s">
@@ -4415,13 +4498,13 @@
         <v>0</v>
       </c>
       <c r="T40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U40" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V40" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W40" s="16">
         <v>0</v>
@@ -4429,38 +4512,38 @@
       <c r="X40" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y40" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z40" t="s">
+      <c r="Y40" s="22">
+        <v>1100100</v>
+      </c>
+      <c r="Z40" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA40" s="13">
-        <v>0</v>
+      <c r="AA40" s="25" t="s">
+        <v>164</v>
       </c>
       <c r="AB40" t="s">
         <v>148</v>
       </c>
       <c r="AC40" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>98</v>
+    <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
       </c>
       <c r="D41" s="10">
-        <v>111001</v>
+        <v>10100</v>
       </c>
       <c r="E41" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x39</v>
+        <v>0x14</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>17</v>
@@ -4474,14 +4557,14 @@
       <c r="I41" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="J41" t="s">
         <v>17</v>
       </c>
       <c r="K41" s="13" t="s">
         <v>17</v>
       </c>
       <c r="L41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="6">
         <v>0</v>
@@ -4493,16 +4576,16 @@
         <v>0</v>
       </c>
       <c r="P41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T41" s="6">
         <v>0</v>
@@ -4519,38 +4602,38 @@
       <c r="X41" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y41" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z41" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA41" s="13">
-        <v>0</v>
+      <c r="Y41" s="22">
+        <v>1100100</v>
+      </c>
+      <c r="Z41" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA41" s="23" t="s">
+        <v>165</v>
       </c>
       <c r="AB41" t="s">
         <v>148</v>
       </c>
       <c r="AC41" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="19" t="s">
+    <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B42" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C42" s="3">
         <v>0</v>
       </c>
       <c r="D42" s="10">
-        <v>1110000</v>
+        <v>10101</v>
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x70</v>
+        <v>0x15</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>17</v>
@@ -4564,17 +4647,17 @@
       <c r="I42" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J42" s="3" t="s">
+      <c r="J42" t="s">
         <v>17</v>
       </c>
       <c r="K42" s="13" t="s">
         <v>17</v>
       </c>
       <c r="L42" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N42" s="6">
         <v>0</v>
@@ -4595,52 +4678,52 @@
         <v>1</v>
       </c>
       <c r="T42" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U42" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V42" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W42" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X42" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y42" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z42" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA42" s="13">
-        <v>0</v>
+      <c r="Y42" s="22">
+        <v>1100100</v>
+      </c>
+      <c r="Z42" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA42" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="AB42" t="s">
         <v>148</v>
       </c>
       <c r="AC42" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="19" t="s">
+    <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
       </c>
       <c r="D43" s="10">
-        <v>1110001</v>
+        <v>10110</v>
       </c>
       <c r="E43" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x71</v>
+        <v>0x16</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>17</v>
@@ -4654,17 +4737,17 @@
       <c r="I43" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="J43" t="s">
         <v>17</v>
       </c>
       <c r="K43" s="13" t="s">
         <v>17</v>
       </c>
       <c r="L43" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N43" s="6">
         <v>0</v>
@@ -4685,52 +4768,52 @@
         <v>1</v>
       </c>
       <c r="T43" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U43" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V43" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W43" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X43" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y43" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA43" s="13">
-        <v>0</v>
+      <c r="Y43" s="22">
+        <v>1100100</v>
+      </c>
+      <c r="Z43" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA43" s="23" t="s">
+        <v>160</v>
       </c>
       <c r="AB43" t="s">
         <v>148</v>
       </c>
       <c r="AC43" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="19" t="s">
+    <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
       </c>
       <c r="D44" s="10">
-        <v>1110010</v>
+        <v>10111</v>
       </c>
       <c r="E44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x72</v>
+        <v>0x17</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>17</v>
@@ -4738,23 +4821,23 @@
       <c r="G44" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" t="s">
         <v>17</v>
       </c>
       <c r="I44" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J44" s="3" t="s">
+      <c r="J44" t="s">
         <v>17</v>
       </c>
       <c r="K44" s="13" t="s">
         <v>17</v>
       </c>
       <c r="L44" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M44" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44" s="6">
         <v>0</v>
@@ -4775,58 +4858,58 @@
         <v>1</v>
       </c>
       <c r="T44" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U44" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V44" s="6">
-        <v>1</v>
-      </c>
-      <c r="W44" s="16">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="W44" s="13">
+        <v>0</v>
       </c>
       <c r="X44" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y44" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z44" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA44" s="13">
-        <v>0</v>
+      <c r="Y44" s="22">
+        <v>1100100</v>
+      </c>
+      <c r="Z44" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA44" s="23" t="s">
+        <v>161</v>
       </c>
       <c r="AB44" t="s">
         <v>148</v>
       </c>
       <c r="AC44" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
       </c>
       <c r="D45" s="10">
-        <v>1110011</v>
+        <v>11010</v>
       </c>
       <c r="E45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x73</v>
+        <v>0x1A</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G45" t="s">
-        <v>17</v>
+        <v>67</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>17</v>
@@ -4841,10 +4924,10 @@
         <v>17</v>
       </c>
       <c r="L45" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" s="6">
         <v>0</v>
@@ -4868,55 +4951,55 @@
         <v>1</v>
       </c>
       <c r="U45" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V45" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W45" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X45" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y45" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z45" t="s">
+      <c r="Y45" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA45" s="13">
+      <c r="AA45" s="23">
         <v>0</v>
       </c>
       <c r="AB45" t="s">
         <v>148</v>
       </c>
       <c r="AC45" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C46" s="3">
         <v>0</v>
       </c>
       <c r="D46" s="10">
-        <v>1110100</v>
+        <v>11100</v>
       </c>
       <c r="E46" s="3" t="str">
-        <f t="shared" ref="E46:E47" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C46,7) + BIN2DEC($D46)))</f>
-        <v>0x74</v>
+        <f t="shared" si="1"/>
+        <v>0x1C</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="G46" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>17</v>
@@ -4931,10 +5014,10 @@
         <v>17</v>
       </c>
       <c r="L46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46" s="6">
         <v>0</v>
@@ -4958,120 +5041,930 @@
         <v>1</v>
       </c>
       <c r="U46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V46" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W46" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X46" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="Y46" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z46" t="s">
+      <c r="Y46" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA46" s="13">
+      <c r="AA46" s="23">
         <v>0</v>
       </c>
       <c r="AB46" t="s">
         <v>148</v>
       </c>
       <c r="AC46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+      <c r="D47" s="10">
+        <v>11101</v>
+      </c>
+      <c r="E47" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x1D</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47" t="s">
+        <v>141</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L47" s="6">
+        <v>0</v>
+      </c>
+      <c r="M47" s="6">
+        <v>0</v>
+      </c>
+      <c r="N47" s="6">
+        <v>0</v>
+      </c>
+      <c r="O47" s="6">
+        <v>0</v>
+      </c>
+      <c r="P47" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="6">
+        <v>1</v>
+      </c>
+      <c r="R47" s="6">
+        <v>1</v>
+      </c>
+      <c r="S47" s="6">
+        <v>1</v>
+      </c>
+      <c r="T47" s="6">
+        <v>1</v>
+      </c>
+      <c r="U47" s="6">
+        <v>0</v>
+      </c>
+      <c r="V47" s="6">
+        <v>0</v>
+      </c>
+      <c r="W47" s="16">
+        <v>0</v>
+      </c>
+      <c r="X47" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y47" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA47" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0</v>
+      </c>
+      <c r="D48" s="10">
+        <v>111010</v>
+      </c>
+      <c r="E48" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x3A</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G48" t="s">
+        <v>141</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L48" s="6">
+        <v>0</v>
+      </c>
+      <c r="M48" s="6">
+        <v>0</v>
+      </c>
+      <c r="N48" s="6">
+        <v>0</v>
+      </c>
+      <c r="O48" s="6">
+        <v>0</v>
+      </c>
+      <c r="P48" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="6">
+        <v>0</v>
+      </c>
+      <c r="R48" s="6">
+        <v>0</v>
+      </c>
+      <c r="S48" s="6">
+        <v>0</v>
+      </c>
+      <c r="T48" s="6">
+        <v>0</v>
+      </c>
+      <c r="U48" s="6">
+        <v>1</v>
+      </c>
+      <c r="V48" s="6">
+        <v>1</v>
+      </c>
+      <c r="W48" s="16">
+        <v>0</v>
+      </c>
+      <c r="X48" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y48" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA48" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0</v>
+      </c>
+      <c r="D49" s="10">
+        <v>111011</v>
+      </c>
+      <c r="E49" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x3B</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" t="s">
+        <v>141</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K49" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L49" s="6">
+        <v>0</v>
+      </c>
+      <c r="M49" s="6">
+        <v>0</v>
+      </c>
+      <c r="N49" s="6">
+        <v>0</v>
+      </c>
+      <c r="O49" s="6">
+        <v>0</v>
+      </c>
+      <c r="P49" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>0</v>
+      </c>
+      <c r="R49" s="6">
+        <v>0</v>
+      </c>
+      <c r="S49" s="6">
+        <v>0</v>
+      </c>
+      <c r="T49" s="6">
+        <v>0</v>
+      </c>
+      <c r="U49" s="6">
+        <v>1</v>
+      </c>
+      <c r="V49" s="6">
+        <v>1</v>
+      </c>
+      <c r="W49" s="16">
+        <v>0</v>
+      </c>
+      <c r="X49" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y49" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA49" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0</v>
+      </c>
+      <c r="D50" s="10">
+        <v>111001</v>
+      </c>
+      <c r="E50" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x39</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L50" s="6">
+        <v>1</v>
+      </c>
+      <c r="M50" s="6">
+        <v>0</v>
+      </c>
+      <c r="N50" s="6">
+        <v>0</v>
+      </c>
+      <c r="O50" s="6">
+        <v>0</v>
+      </c>
+      <c r="P50" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="6">
+        <v>0</v>
+      </c>
+      <c r="R50" s="6">
+        <v>0</v>
+      </c>
+      <c r="S50" s="6">
+        <v>0</v>
+      </c>
+      <c r="T50" s="6">
+        <v>0</v>
+      </c>
+      <c r="U50" s="6">
+        <v>0</v>
+      </c>
+      <c r="V50" s="6">
+        <v>0</v>
+      </c>
+      <c r="W50" s="16">
+        <v>0</v>
+      </c>
+      <c r="X50" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y50" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA50" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0</v>
+      </c>
+      <c r="D51" s="10">
+        <v>1110000</v>
+      </c>
+      <c r="E51" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x70</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K51" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L51" s="6">
+        <v>1</v>
+      </c>
+      <c r="M51" s="6">
+        <v>1</v>
+      </c>
+      <c r="N51" s="6">
+        <v>0</v>
+      </c>
+      <c r="O51" s="6">
+        <v>0</v>
+      </c>
+      <c r="P51" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>1</v>
+      </c>
+      <c r="R51" s="6">
+        <v>1</v>
+      </c>
+      <c r="S51" s="6">
+        <v>1</v>
+      </c>
+      <c r="T51" s="6">
+        <v>1</v>
+      </c>
+      <c r="U51" s="6">
+        <v>1</v>
+      </c>
+      <c r="V51" s="6">
+        <v>1</v>
+      </c>
+      <c r="W51" s="16">
+        <v>1</v>
+      </c>
+      <c r="X51" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y51" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA51" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0</v>
+      </c>
+      <c r="D52" s="10">
+        <v>1110001</v>
+      </c>
+      <c r="E52" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x71</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K52" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L52" s="6">
+        <v>1</v>
+      </c>
+      <c r="M52" s="6">
+        <v>1</v>
+      </c>
+      <c r="N52" s="6">
+        <v>0</v>
+      </c>
+      <c r="O52" s="6">
+        <v>0</v>
+      </c>
+      <c r="P52" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>1</v>
+      </c>
+      <c r="R52" s="6">
+        <v>1</v>
+      </c>
+      <c r="S52" s="6">
+        <v>1</v>
+      </c>
+      <c r="T52" s="6">
+        <v>1</v>
+      </c>
+      <c r="U52" s="6">
+        <v>1</v>
+      </c>
+      <c r="V52" s="6">
+        <v>1</v>
+      </c>
+      <c r="W52" s="16">
+        <v>1</v>
+      </c>
+      <c r="X52" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y52" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA52" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="3">
+        <v>0</v>
+      </c>
+      <c r="D53" s="10">
+        <v>1110010</v>
+      </c>
+      <c r="E53" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x72</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K53" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L53" s="6">
+        <v>1</v>
+      </c>
+      <c r="M53" s="6">
+        <v>1</v>
+      </c>
+      <c r="N53" s="6">
+        <v>0</v>
+      </c>
+      <c r="O53" s="6">
+        <v>0</v>
+      </c>
+      <c r="P53" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="6">
+        <v>1</v>
+      </c>
+      <c r="R53" s="6">
+        <v>1</v>
+      </c>
+      <c r="S53" s="6">
+        <v>1</v>
+      </c>
+      <c r="T53" s="6">
+        <v>1</v>
+      </c>
+      <c r="U53" s="6">
+        <v>1</v>
+      </c>
+      <c r="V53" s="6">
+        <v>1</v>
+      </c>
+      <c r="W53" s="16">
+        <v>1</v>
+      </c>
+      <c r="X53" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y53" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA53" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0</v>
+      </c>
+      <c r="D54" s="10">
+        <v>1110011</v>
+      </c>
+      <c r="E54" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x73</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K54" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L54" s="6">
+        <v>1</v>
+      </c>
+      <c r="M54" s="6">
+        <v>1</v>
+      </c>
+      <c r="N54" s="6">
+        <v>0</v>
+      </c>
+      <c r="O54" s="6">
+        <v>0</v>
+      </c>
+      <c r="P54" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>1</v>
+      </c>
+      <c r="R54" s="6">
+        <v>1</v>
+      </c>
+      <c r="S54" s="6">
+        <v>1</v>
+      </c>
+      <c r="T54" s="6">
+        <v>1</v>
+      </c>
+      <c r="U54" s="6">
+        <v>1</v>
+      </c>
+      <c r="V54" s="6">
+        <v>1</v>
+      </c>
+      <c r="W54" s="16">
+        <v>1</v>
+      </c>
+      <c r="X54" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y54" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA54" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0</v>
+      </c>
+      <c r="D55" s="10">
+        <v>1110100</v>
+      </c>
+      <c r="E55" s="3" t="str">
+        <f t="shared" ref="E55:E56" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C55,7) + BIN2DEC($D55)))</f>
+        <v>0x74</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G55" t="s">
+        <v>17</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K55" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L55" s="6">
+        <v>1</v>
+      </c>
+      <c r="M55" s="6">
+        <v>1</v>
+      </c>
+      <c r="N55" s="6">
+        <v>0</v>
+      </c>
+      <c r="O55" s="6">
+        <v>0</v>
+      </c>
+      <c r="P55" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="6">
+        <v>1</v>
+      </c>
+      <c r="R55" s="6">
+        <v>1</v>
+      </c>
+      <c r="S55" s="6">
+        <v>1</v>
+      </c>
+      <c r="T55" s="6">
+        <v>1</v>
+      </c>
+      <c r="U55" s="6">
+        <v>1</v>
+      </c>
+      <c r="V55" s="6">
+        <v>1</v>
+      </c>
+      <c r="W55" s="16">
+        <v>1</v>
+      </c>
+      <c r="X55" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y55" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z55" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA55" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC55" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+    <row r="56" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B56" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="3">
-        <v>0</v>
-      </c>
-      <c r="D47" s="10">
+      <c r="C56" s="3">
+        <v>0</v>
+      </c>
+      <c r="D56" s="10">
         <v>1111000</v>
       </c>
-      <c r="E47" s="3" t="str">
+      <c r="E56" s="3" t="str">
         <f t="shared" si="2"/>
         <v>0x78</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G47" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K47" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L47" s="6">
-        <v>1</v>
-      </c>
-      <c r="M47" s="6">
-        <v>1</v>
-      </c>
-      <c r="N47" s="6">
-        <v>0</v>
-      </c>
-      <c r="O47" s="6">
-        <v>0</v>
-      </c>
-      <c r="P47" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q47" s="6">
-        <v>1</v>
-      </c>
-      <c r="R47" s="6">
-        <v>1</v>
-      </c>
-      <c r="S47" s="6">
-        <v>1</v>
-      </c>
-      <c r="T47" s="6">
-        <v>1</v>
-      </c>
-      <c r="U47" s="6">
-        <v>1</v>
-      </c>
-      <c r="V47" s="6">
-        <v>1</v>
-      </c>
-      <c r="W47" s="16">
-        <v>1</v>
-      </c>
-      <c r="X47" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y47" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z47" t="s">
+      <c r="F56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K56" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L56" s="6">
+        <v>1</v>
+      </c>
+      <c r="M56" s="6">
+        <v>1</v>
+      </c>
+      <c r="N56" s="6">
+        <v>0</v>
+      </c>
+      <c r="O56" s="6">
+        <v>0</v>
+      </c>
+      <c r="P56" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="6">
+        <v>1</v>
+      </c>
+      <c r="R56" s="6">
+        <v>1</v>
+      </c>
+      <c r="S56" s="6">
+        <v>1</v>
+      </c>
+      <c r="T56" s="6">
+        <v>1</v>
+      </c>
+      <c r="U56" s="6">
+        <v>1</v>
+      </c>
+      <c r="V56" s="6">
+        <v>1</v>
+      </c>
+      <c r="W56" s="16">
+        <v>1</v>
+      </c>
+      <c r="X56" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y56" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA47" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB47" t="s">
+      <c r="AA56" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB56" t="s">
         <v>148</v>
       </c>
-      <c r="AC47" t="s">
+      <c r="AC56" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing typo in write value
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F39F2B-2968-2F4E-B6E0-EF1F60DD085E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049EA7EC-EA1E-EC49-A733-81EB5F8E1809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -513,31 +513,31 @@
     <t>set_can_run</t>
   </si>
   <si>
-    <t>0x3c3c0100010101013c3c3c</t>
-  </si>
-  <si>
-    <t>0x3c3c0100020202023c3c3c</t>
-  </si>
-  <si>
-    <t>0x3c3c0100030303033c3c3c</t>
-  </si>
-  <si>
-    <t>0x3c3c0100040404043c3c3c</t>
-  </si>
-  <si>
-    <t>0x3c3c0100050505053c3c3c</t>
-  </si>
-  <si>
-    <t>0x3c3c0100060606063c3c3c</t>
-  </si>
-  <si>
-    <t>0x3c3c0100000000003c3c3c</t>
-  </si>
-  <si>
     <t>set the DE mode</t>
   </si>
   <si>
     <t>set the canister mode</t>
+  </si>
+  <si>
+    <t>0x3c3c0100010101013c3c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100020202023c3c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100030303033c3c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100040404043c3c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100050505053c3c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100060606063c3c3c3c</t>
+  </si>
+  <si>
+    <t>0x3c3c0100000000003c3c3c3c</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1012,10 @@
   <dimension ref="A1:AC56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="M21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomRight" activeCell="AA45" sqref="AA45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1036,7 @@
     <col min="24" max="24" width="10.83203125" style="13"/>
     <col min="25" max="25" width="12.83203125" style="20" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.6640625" style="21" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19.1640625" customWidth="1"/>
     <col min="29" max="29" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4069,7 +4069,7 @@
         <v>74</v>
       </c>
       <c r="AA35" s="23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AB35" t="s">
         <v>148</v>
@@ -4159,13 +4159,13 @@
         <v>74</v>
       </c>
       <c r="AA36" s="23" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AB36" t="s">
         <v>148</v>
       </c>
       <c r="AC36" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4249,13 +4249,13 @@
         <v>74</v>
       </c>
       <c r="AA37" s="25" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AB37" t="s">
         <v>148</v>
       </c>
       <c r="AC37" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4339,13 +4339,13 @@
         <v>74</v>
       </c>
       <c r="AA38" s="25" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="AB38" t="s">
         <v>148</v>
       </c>
       <c r="AC38" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4429,13 +4429,13 @@
         <v>74</v>
       </c>
       <c r="AA39" s="25" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="AB39" t="s">
         <v>148</v>
       </c>
       <c r="AC39" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4519,13 +4519,13 @@
         <v>74</v>
       </c>
       <c r="AA40" s="25" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AB40" t="s">
         <v>148</v>
       </c>
       <c r="AC40" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4609,13 +4609,13 @@
         <v>154</v>
       </c>
       <c r="AA41" s="23" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="AB41" t="s">
         <v>148</v>
       </c>
       <c r="AC41" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4699,13 +4699,13 @@
         <v>154</v>
       </c>
       <c r="AA42" s="23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AB42" t="s">
         <v>148</v>
       </c>
       <c r="AC42" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4789,13 +4789,13 @@
         <v>154</v>
       </c>
       <c r="AA43" s="23" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AB43" t="s">
         <v>148</v>
       </c>
       <c r="AC43" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4879,13 +4879,13 @@
         <v>154</v>
       </c>
       <c r="AA44" s="23" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AB44" t="s">
         <v>148</v>
       </c>
       <c r="AC44" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adding a read command to DE deck
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049EA7EC-EA1E-EC49-A733-81EB5F8E1809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E371FC-90DC-A547-A436-8634A741708B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -1012,10 +1012,10 @@
   <dimension ref="A1:AC56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="M21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA45" sqref="AA45"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1890,7 @@
       </c>
     </row>
     <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="19" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="18" t="s">
@@ -1964,13 +1964,13 @@
         <v>141</v>
       </c>
       <c r="Y11" s="22">
-        <v>0</v>
+        <v>1100100</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>74</v>
       </c>
       <c r="AA11" s="23">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AB11" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
changing length field to hex for read commands
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E371FC-90DC-A547-A436-8634A741708B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F079B5F-1791-7D45-A065-B343FCDD159D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="169">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -538,6 +538,9 @@
   </si>
   <si>
     <t>0x3c3c0100000000003c3c3c3c</t>
+  </si>
+  <si>
+    <t>0x0C</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1018,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1969,8 +1972,8 @@
       <c r="Z11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AA11" s="23">
-        <v>12</v>
+      <c r="AA11" s="23" t="s">
+        <v>168</v>
       </c>
       <c r="AB11" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
using reply.length [B] field to indicate reply length, and renamed old reply field to . It now holds the hex value that should be written to memory for each write command.
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F079B5F-1791-7D45-A065-B343FCDD159D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E1A0C5-DA16-A346-823A-DA3C8D4DC6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="176">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -255,9 +255,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>length</t>
-  </si>
-  <si>
     <t>0x00</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>hk</t>
   </si>
   <si>
-    <t>see lookup</t>
-  </si>
-  <si>
     <t>temp</t>
   </si>
   <si>
@@ -540,7 +534,34 @@
     <t>0x3c3c0100000000003c3c3c3c</t>
   </si>
   <si>
-    <t>0x0C</t>
+    <t>0x0c</t>
+  </si>
+  <si>
+    <t>read_ring_wr_ptr</t>
+  </si>
+  <si>
+    <t>wr_ptr</t>
+  </si>
+  <si>
+    <t>0x022b0308</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>write_value</t>
+  </si>
+  <si>
+    <t>0x022b02fc</t>
   </si>
 </sst>
 </file>
@@ -644,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -696,6 +717,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1012,13 +1041,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC56"/>
+  <dimension ref="A1:AC57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA11" sqref="AA11"/>
+      <selection pane="bottomRight" activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1092,7 @@
       </c>
       <c r="K1" s="27"/>
       <c r="L1" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
@@ -1078,7 +1107,7 @@
       <c r="W1" s="27"/>
       <c r="X1" s="12"/>
       <c r="Y1" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Z1" s="27"/>
       <c r="AA1" s="28"/>
@@ -1121,7 +1150,7 @@
         <v>7</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>8</v>
@@ -1130,25 +1159,25 @@
         <v>9</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="W2" s="15" t="s">
         <v>10</v>
@@ -1163,7 +1192,7 @@
         <v>72</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>12</v>
@@ -1177,7 +1206,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -1186,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E23" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
+        <f t="shared" ref="E3:E24" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
         <v>0x80</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1204,8 +1233,8 @@
       <c r="J3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="13">
-        <v>1</v>
+      <c r="K3" s="23" t="s">
+        <v>173</v>
       </c>
       <c r="L3" s="6">
         <v>0</v>
@@ -1244,22 +1273,22 @@
         <v>1</v>
       </c>
       <c r="X3" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y3" s="22">
         <v>0</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA3" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA3" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="AB3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -1267,7 +1296,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -1294,8 +1323,8 @@
       <c r="J4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="13">
-        <v>1</v>
+      <c r="K4" s="23" t="s">
+        <v>173</v>
       </c>
       <c r="L4" s="6">
         <v>0</v>
@@ -1334,22 +1363,22 @@
         <v>0</v>
       </c>
       <c r="X4" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y4" s="22">
         <v>0</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA4" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA4" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="AB4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -1357,7 +1386,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -1384,8 +1413,8 @@
       <c r="J5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="13" t="s">
-        <v>5</v>
+      <c r="K5" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -1424,22 +1453,22 @@
         <v>0</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y5" s="22">
         <v>0</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA5" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA5" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="AB5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -1447,7 +1476,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -1472,10 +1501,10 @@
         <v>17</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L6" s="6">
         <v>1</v>
@@ -1514,22 +1543,22 @@
         <v>1</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y6" s="22">
         <v>0</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA6" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA6" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="AB6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -1537,7 +1566,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -1562,10 +1591,10 @@
         <v>17</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L7" s="6">
         <v>1</v>
@@ -1604,22 +1633,22 @@
         <v>1</v>
       </c>
       <c r="X7" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y7" s="22">
         <v>0</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA7" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA7" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="AB7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -1627,7 +1656,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -1654,8 +1683,8 @@
       <c r="J8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="13" t="s">
-        <v>79</v>
+      <c r="K8" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L8" s="6">
         <v>1</v>
@@ -1694,22 +1723,22 @@
         <v>1</v>
       </c>
       <c r="X8" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y8" s="22">
         <v>0</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA8" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA8" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="AB8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -1717,7 +1746,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -1742,11 +1771,11 @@
         <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K9" s="13" t="s">
         <v>79</v>
       </c>
+      <c r="K9" s="23" t="s">
+        <v>73</v>
+      </c>
       <c r="L9" s="6">
         <v>1</v>
       </c>
@@ -1784,130 +1813,127 @@
         <v>1</v>
       </c>
       <c r="X9" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y9" s="22">
         <v>0</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA9" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA9" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="AB9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
+    <row r="10" spans="1:29" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>167</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="10">
-        <v>11000</v>
+        <v>1110</v>
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x98</v>
+        <v>0x8E</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="29" t="s">
         <v>17</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="30" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
-      <c r="O10" s="6">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>1</v>
-      </c>
-      <c r="R10" s="6">
-        <v>1</v>
-      </c>
-      <c r="S10" s="6">
-        <v>1</v>
-      </c>
-      <c r="T10" s="6">
-        <v>1</v>
-      </c>
-      <c r="U10" s="6">
-        <v>0</v>
-      </c>
-      <c r="V10" s="6">
-        <v>0</v>
-      </c>
-      <c r="W10" s="16">
-        <v>0</v>
-      </c>
-      <c r="X10" s="13" t="s">
-        <v>141</v>
+        <v>168</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="L10" s="31">
+        <v>0</v>
+      </c>
+      <c r="M10" s="31">
+        <v>0</v>
+      </c>
+      <c r="N10" s="31">
+        <v>0</v>
+      </c>
+      <c r="O10" s="31">
+        <v>0</v>
+      </c>
+      <c r="P10" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="31">
+        <v>1</v>
+      </c>
+      <c r="R10" s="31">
+        <v>1</v>
+      </c>
+      <c r="S10" s="31">
+        <v>1</v>
+      </c>
+      <c r="T10" s="31">
+        <v>0</v>
+      </c>
+      <c r="U10" s="31">
+        <v>0</v>
+      </c>
+      <c r="V10" s="31">
+        <v>0</v>
+      </c>
+      <c r="W10" s="32">
+        <v>0</v>
+      </c>
+      <c r="X10" s="30" t="s">
+        <v>139</v>
       </c>
       <c r="Y10" s="22">
         <v>0</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA10" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>148</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>108</v>
+        <v>169</v>
+      </c>
+      <c r="AA10" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB10" s="29" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>31</v>
+      <c r="A11" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" s="10">
-        <v>11010</v>
+        <v>11000</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x9A</v>
+        <v>0x98</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>17</v>
@@ -1922,10 +1948,10 @@
         <v>17</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L11" s="6">
         <v>0</v>
@@ -1964,40 +1990,40 @@
         <v>0</v>
       </c>
       <c r="X11" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y11" s="22">
-        <v>1100100</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA11" s="23" t="s">
-        <v>168</v>
+        <v>73</v>
       </c>
       <c r="AB11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>32</v>
+      <c r="A12" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" s="10">
-        <v>11100</v>
+        <v>11010</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x9C</v>
+        <v>0x9A</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>17</v>
@@ -2012,10 +2038,10 @@
         <v>17</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>166</v>
       </c>
       <c r="L12" s="6">
         <v>0</v>
@@ -2054,40 +2080,40 @@
         <v>0</v>
       </c>
       <c r="X12" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y12" s="22">
-        <v>0</v>
+        <v>1100100</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA12" s="23">
-        <v>0</v>
+        <v>175</v>
+      </c>
+      <c r="AA12" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="10">
-        <v>11101</v>
+        <v>11100</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x9D</v>
+        <v>0x9C</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>17</v>
@@ -2102,10 +2128,10 @@
         <v>17</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="13">
-        <v>8</v>
+        <v>81</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L13" s="6">
         <v>0</v>
@@ -2144,40 +2170,40 @@
         <v>0</v>
       </c>
       <c r="X13" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y13" s="22">
         <v>0</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA13" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA13" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" s="10">
-        <v>100001</v>
+        <v>11101</v>
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xA1</v>
+        <v>0x9D</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
@@ -2192,10 +2218,10 @@
         <v>17</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" s="13">
-        <v>2</v>
+        <v>82</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>170</v>
       </c>
       <c r="L14" s="6">
         <v>0</v>
@@ -2231,43 +2257,43 @@
         <v>0</v>
       </c>
       <c r="W14" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X14" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y14" s="22">
         <v>0</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA14" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA14" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="10">
-        <v>100100</v>
+        <v>100001</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xA4</v>
+        <v>0xA1</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>17</v>
@@ -2282,16 +2308,16 @@
         <v>17</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>141</v>
+        <v>70</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>171</v>
       </c>
       <c r="L15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="6">
         <v>0</v>
@@ -2315,49 +2341,49 @@
         <v>1</v>
       </c>
       <c r="U15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15" s="16">
         <v>1</v>
       </c>
       <c r="X15" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y15" s="22">
         <v>0</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA15" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA15" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>97</v>
-      </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" s="10">
-        <v>101000</v>
+        <v>100100</v>
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xA8</v>
+        <v>0xA4</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>17</v>
@@ -2372,16 +2398,16 @@
         <v>17</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>141</v>
+        <v>83</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L16" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="6">
         <v>0</v>
@@ -2405,49 +2431,49 @@
         <v>1</v>
       </c>
       <c r="U16" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W16" s="16">
         <v>1</v>
       </c>
       <c r="X16" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y16" s="22">
         <v>0</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA16" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA16" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC16" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
       </c>
       <c r="D17" s="10">
-        <v>10010</v>
+        <v>101000</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x92</v>
+        <v>0xA8</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>17</v>
@@ -2462,10 +2488,10 @@
         <v>17</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>141</v>
+        <v>94</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L17" s="6">
         <v>0</v>
@@ -2480,64 +2506,64 @@
         <v>0</v>
       </c>
       <c r="P17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X17" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y17" s="22">
         <v>0</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA17" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA17" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC17" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
       </c>
       <c r="D18" s="10">
-        <v>10011</v>
+        <v>10010</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x93</v>
+        <v>0x92</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>17</v>
@@ -2552,10 +2578,10 @@
         <v>17</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>141</v>
+        <v>84</v>
+      </c>
+      <c r="K18" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L18" s="6">
         <v>0</v>
@@ -2594,40 +2620,40 @@
         <v>0</v>
       </c>
       <c r="X18" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y18" s="22">
         <v>0</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA18" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA18" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
       </c>
       <c r="D19" s="10">
-        <v>111000</v>
+        <v>10011</v>
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xB8</v>
+        <v>0x93</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>17</v>
@@ -2642,13 +2668,13 @@
         <v>17</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K19" s="13">
-        <v>2</v>
+        <v>84</v>
+      </c>
+      <c r="K19" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="6">
         <v>0</v>
@@ -2675,49 +2701,49 @@
         <v>0</v>
       </c>
       <c r="U19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19" s="16">
         <v>0</v>
       </c>
       <c r="X19" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y19" s="22">
         <v>0</v>
       </c>
       <c r="Z19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA19" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA19" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC19" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
       </c>
       <c r="D20" s="10">
-        <v>110101</v>
+        <v>111000</v>
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xB5</v>
+        <v>0xB8</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>17</v>
@@ -2732,16 +2758,16 @@
         <v>17</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="K20" s="13">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="K20" s="23" t="s">
+        <v>171</v>
       </c>
       <c r="L20" s="6">
         <v>1</v>
       </c>
       <c r="M20" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20" s="6">
         <v>0</v>
@@ -2774,40 +2800,40 @@
         <v>0</v>
       </c>
       <c r="X20" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y20" s="22">
         <v>0</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA20" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA20" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC20" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
       </c>
       <c r="D21" s="10">
-        <v>110110</v>
+        <v>110101</v>
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xB6</v>
+        <v>0xB5</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>17</v>
@@ -2822,10 +2848,10 @@
         <v>17</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K21" s="13">
-        <v>1</v>
+        <v>141</v>
+      </c>
+      <c r="K21" s="23" t="s">
+        <v>172</v>
       </c>
       <c r="L21" s="6">
         <v>1</v>
@@ -2864,40 +2890,40 @@
         <v>0</v>
       </c>
       <c r="X21" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y21" s="22">
         <v>0</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA21" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA21" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
       </c>
       <c r="D22" s="10">
-        <v>110111</v>
+        <v>110110</v>
       </c>
       <c r="E22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xB7</v>
+        <v>0xB6</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>17</v>
@@ -2912,10 +2938,10 @@
         <v>17</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="K22" s="13">
-        <v>2</v>
+        <v>140</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>172</v>
       </c>
       <c r="L22" s="6">
         <v>1</v>
@@ -2954,248 +2980,248 @@
         <v>0</v>
       </c>
       <c r="X22" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y22" s="22">
         <v>0</v>
       </c>
       <c r="Z22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA22" s="23">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="AA22" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="AB22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
       </c>
       <c r="D23" s="10">
-        <v>111001</v>
+        <v>110111</v>
       </c>
       <c r="E23" s="3" t="str">
         <f t="shared" si="0"/>
+        <v>0xB7</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K23" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="L23" s="6">
+        <v>1</v>
+      </c>
+      <c r="M23" s="6">
+        <v>1</v>
+      </c>
+      <c r="N23" s="6">
+        <v>0</v>
+      </c>
+      <c r="O23" s="6">
+        <v>0</v>
+      </c>
+      <c r="P23" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="6">
+        <v>0</v>
+      </c>
+      <c r="R23" s="6">
+        <v>0</v>
+      </c>
+      <c r="S23" s="6">
+        <v>0</v>
+      </c>
+      <c r="T23" s="6">
+        <v>0</v>
+      </c>
+      <c r="U23" s="6">
+        <v>0</v>
+      </c>
+      <c r="V23" s="6">
+        <v>0</v>
+      </c>
+      <c r="W23" s="16">
+        <v>0</v>
+      </c>
+      <c r="X23" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y23" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA23" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="10">
+        <v>111001</v>
+      </c>
+      <c r="E24" s="3" t="str">
+        <f t="shared" si="0"/>
         <v>0xB9</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K23" s="13">
-        <v>1</v>
-      </c>
-      <c r="L23" s="6">
-        <v>1</v>
-      </c>
-      <c r="M23" s="6">
-        <v>0</v>
-      </c>
-      <c r="N23" s="6">
-        <v>0</v>
-      </c>
-      <c r="O23" s="6">
-        <v>0</v>
-      </c>
-      <c r="P23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="6">
-        <v>0</v>
-      </c>
-      <c r="R23" s="6">
-        <v>0</v>
-      </c>
-      <c r="S23" s="6">
-        <v>0</v>
-      </c>
-      <c r="T23" s="6">
-        <v>0</v>
-      </c>
-      <c r="U23" s="6">
-        <v>0</v>
-      </c>
-      <c r="V23" s="6">
-        <v>0</v>
-      </c>
-      <c r="W23" s="16">
-        <v>0</v>
-      </c>
-      <c r="X23" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y23" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA23" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>148</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>119</v>
+      <c r="F24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="L24" s="6">
+        <v>1</v>
+      </c>
+      <c r="M24" s="6">
+        <v>0</v>
+      </c>
+      <c r="N24" s="6">
+        <v>0</v>
+      </c>
+      <c r="O24" s="6">
+        <v>0</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>0</v>
+      </c>
+      <c r="R24" s="6">
+        <v>0</v>
+      </c>
+      <c r="S24" s="6">
+        <v>0</v>
+      </c>
+      <c r="T24" s="6">
+        <v>0</v>
+      </c>
+      <c r="U24" s="6">
+        <v>0</v>
+      </c>
+      <c r="V24" s="6">
+        <v>0</v>
+      </c>
+      <c r="W24" s="16">
+        <v>0</v>
+      </c>
+      <c r="X24" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y24" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA24" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="17"/>
-      <c r="X24" s="14"/>
-      <c r="Y24" s="24"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="24"/>
-    </row>
-    <row r="25" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="10">
-        <v>1000000</v>
-      </c>
-      <c r="E25" s="3" t="str">
-        <f t="shared" ref="E25:E54" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C25,7) + BIN2DEC($D25)))</f>
-        <v>0x40</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L25" s="6">
-        <v>0</v>
-      </c>
-      <c r="M25" s="6">
-        <v>1</v>
-      </c>
-      <c r="N25" s="6">
-        <v>0</v>
-      </c>
-      <c r="O25" s="6">
-        <v>0</v>
-      </c>
-      <c r="P25" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="6">
-        <v>0</v>
-      </c>
-      <c r="R25" s="6">
-        <v>0</v>
-      </c>
-      <c r="S25" s="6">
-        <v>0</v>
-      </c>
-      <c r="T25" s="6">
-        <v>0</v>
-      </c>
-      <c r="U25" s="6">
-        <v>0</v>
-      </c>
-      <c r="V25" s="6">
-        <v>0</v>
-      </c>
-      <c r="W25" s="16">
-        <v>0</v>
-      </c>
-      <c r="X25" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y25" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA25" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>148</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>120</v>
-      </c>
+    <row r="25" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="24"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="24"/>
     </row>
     <row r="26" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <v>1000010</v>
+        <v>1000000</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x42</v>
+        <f t="shared" ref="E26:E55" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C26,7) + BIN2DEC($D26)))</f>
+        <v>0x40</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>69</v>
@@ -3212,8 +3238,8 @@
       <c r="J26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="13" t="s">
-        <v>17</v>
+      <c r="K26" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L26" s="6">
         <v>0</v>
@@ -3252,46 +3278,46 @@
         <v>0</v>
       </c>
       <c r="X26" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y26" s="22">
         <v>0</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA26" s="23">
         <v>0</v>
       </c>
       <c r="AB26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
       </c>
       <c r="D27" s="10">
-        <v>1000100</v>
+        <v>1000010</v>
       </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x44</v>
+        <v>0x42</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" t="s">
-        <v>17</v>
+        <v>69</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>17</v>
@@ -3302,14 +3328,14 @@
       <c r="J27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="13" t="s">
-        <v>17</v>
+      <c r="K27" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L27" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" s="6">
         <v>0</v>
@@ -3342,40 +3368,40 @@
         <v>0</v>
       </c>
       <c r="X27" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y27" s="22">
         <v>0</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA27" s="23">
         <v>0</v>
       </c>
       <c r="AB27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC27" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
       </c>
       <c r="D28" s="10">
-        <v>1000101</v>
+        <v>1000100</v>
       </c>
       <c r="E28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x45</v>
+        <v>0x44</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>17</v>
@@ -3392,8 +3418,8 @@
       <c r="J28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="13" t="s">
-        <v>17</v>
+      <c r="K28" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L28" s="6">
         <v>1</v>
@@ -3432,46 +3458,46 @@
         <v>0</v>
       </c>
       <c r="X28" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y28" s="22">
         <v>0</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA28" s="23">
         <v>0</v>
       </c>
       <c r="AB28" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
       </c>
       <c r="D29" s="10">
-        <v>1110111</v>
+        <v>1000101</v>
       </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x77</v>
+        <v>0x45</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G29" t="s">
+        <v>17</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>17</v>
@@ -3482,8 +3508,8 @@
       <c r="J29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="13" t="s">
-        <v>17</v>
+      <c r="K29" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L29" s="6">
         <v>1</v>
@@ -3522,43 +3548,43 @@
         <v>0</v>
       </c>
       <c r="X29" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y29" s="22">
         <v>0</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA29" s="23">
         <v>0</v>
       </c>
       <c r="AB29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC29" t="s">
-        <v>122</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
       </c>
       <c r="D30" s="10">
-        <v>1100001</v>
+        <v>1110111</v>
       </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x61</v>
+        <v>0x77</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G30">
         <v>2</v>
@@ -3572,11 +3598,11 @@
       <c r="J30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="13" t="s">
-        <v>17</v>
+      <c r="K30" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L30" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="6">
         <v>0</v>
@@ -3588,19 +3614,19 @@
         <v>0</v>
       </c>
       <c r="P30" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R30" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S30" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T30" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U30" s="6">
         <v>0</v>
@@ -3609,49 +3635,49 @@
         <v>0</v>
       </c>
       <c r="W30" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X30" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y30" s="22">
         <v>0</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA30" s="23">
         <v>0</v>
       </c>
       <c r="AB30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC30" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
       </c>
       <c r="D31" s="10">
-        <v>1100010</v>
+        <v>1100001</v>
       </c>
       <c r="E31" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x62</v>
+        <v>0x61</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" t="s">
-        <v>17</v>
+        <v>70</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>17</v>
@@ -3662,8 +3688,8 @@
       <c r="J31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="13" t="s">
-        <v>17</v>
+      <c r="K31" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L31" s="6">
         <v>0</v>
@@ -3702,40 +3728,40 @@
         <v>1</v>
       </c>
       <c r="X31" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y31" s="22">
         <v>0</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA31" s="23">
         <v>0</v>
       </c>
       <c r="AB31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
       </c>
       <c r="D32" s="10">
-        <v>1100011</v>
+        <v>1100010</v>
       </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x63</v>
+        <v>0x62</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>17</v>
@@ -3752,8 +3778,8 @@
       <c r="J32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="13" t="s">
-        <v>17</v>
+      <c r="K32" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L32" s="6">
         <v>0</v>
@@ -3792,40 +3818,40 @@
         <v>1</v>
       </c>
       <c r="X32" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y32" s="22">
         <v>0</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA32" s="23">
         <v>0</v>
       </c>
       <c r="AB32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" s="3">
         <v>0</v>
       </c>
       <c r="D33" s="10">
-        <v>100100</v>
+        <v>1100011</v>
       </c>
       <c r="E33" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x24</v>
+        <v>0x63</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>17</v>
@@ -3842,14 +3868,14 @@
       <c r="J33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="13" t="s">
-        <v>17</v>
+      <c r="K33" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L33" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" s="6">
         <v>0</v>
@@ -3873,248 +3899,248 @@
         <v>1</v>
       </c>
       <c r="U33" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V33" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W33" s="16">
         <v>1</v>
       </c>
       <c r="X33" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y33" s="22">
         <v>0</v>
       </c>
       <c r="Z33" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA33" s="23">
         <v>0</v>
       </c>
       <c r="AB33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC33" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
       </c>
       <c r="D34" s="10">
-        <v>100101</v>
+        <v>100100</v>
       </c>
       <c r="E34" s="3" t="str">
         <f t="shared" si="1"/>
+        <v>0x24</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K34" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="L34" s="6">
+        <v>1</v>
+      </c>
+      <c r="M34" s="6">
+        <v>1</v>
+      </c>
+      <c r="N34" s="6">
+        <v>0</v>
+      </c>
+      <c r="O34" s="6">
+        <v>0</v>
+      </c>
+      <c r="P34" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="6">
+        <v>1</v>
+      </c>
+      <c r="R34" s="6">
+        <v>1</v>
+      </c>
+      <c r="S34" s="6">
+        <v>1</v>
+      </c>
+      <c r="T34" s="6">
+        <v>1</v>
+      </c>
+      <c r="U34" s="6">
+        <v>1</v>
+      </c>
+      <c r="V34" s="6">
+        <v>1</v>
+      </c>
+      <c r="W34" s="16">
+        <v>1</v>
+      </c>
+      <c r="X34" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y34" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA34" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10">
+        <v>100101</v>
+      </c>
+      <c r="E35" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>0x25</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L34" s="6">
-        <v>1</v>
-      </c>
-      <c r="M34" s="6">
-        <v>1</v>
-      </c>
-      <c r="N34" s="6">
-        <v>0</v>
-      </c>
-      <c r="O34" s="6">
-        <v>0</v>
-      </c>
-      <c r="P34" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="6">
-        <v>1</v>
-      </c>
-      <c r="R34" s="6">
-        <v>1</v>
-      </c>
-      <c r="S34" s="6">
-        <v>1</v>
-      </c>
-      <c r="T34" s="6">
-        <v>1</v>
-      </c>
-      <c r="U34" s="6">
-        <v>1</v>
-      </c>
-      <c r="V34" s="6">
-        <v>1</v>
-      </c>
-      <c r="W34" s="16">
-        <v>1</v>
-      </c>
-      <c r="X34" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y34" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA34" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>148</v>
-      </c>
-      <c r="AC34" t="s">
-        <v>127</v>
+      <c r="F35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="L35" s="6">
+        <v>1</v>
+      </c>
+      <c r="M35" s="6">
+        <v>1</v>
+      </c>
+      <c r="N35" s="6">
+        <v>0</v>
+      </c>
+      <c r="O35" s="6">
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>1</v>
+      </c>
+      <c r="R35" s="6">
+        <v>1</v>
+      </c>
+      <c r="S35" s="6">
+        <v>1</v>
+      </c>
+      <c r="T35" s="6">
+        <v>1</v>
+      </c>
+      <c r="U35" s="6">
+        <v>1</v>
+      </c>
+      <c r="V35" s="6">
+        <v>1</v>
+      </c>
+      <c r="W35" s="16">
+        <v>1</v>
+      </c>
+      <c r="X35" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y35" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA35" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+    <row r="36" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="10">
+      <c r="B36" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10">
         <v>11000</v>
       </c>
-      <c r="E35" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C35,7) + BIN2DEC($D35)))</f>
+      <c r="E36" s="3" t="str">
+        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C36,7) + BIN2DEC($D36)))</f>
         <v>0x18</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="I35" s="13">
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I36" s="13">
         <f>68*2</f>
         <v>136</v>
       </c>
-      <c r="J35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K35" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L35" s="6">
-        <v>0</v>
-      </c>
-      <c r="M35" s="6">
-        <v>0</v>
-      </c>
-      <c r="N35" s="6">
-        <v>0</v>
-      </c>
-      <c r="O35" s="6">
-        <v>0</v>
-      </c>
-      <c r="P35" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="6">
-        <v>1</v>
-      </c>
-      <c r="R35" s="6">
-        <v>1</v>
-      </c>
-      <c r="S35" s="6">
-        <v>1</v>
-      </c>
-      <c r="T35" s="6">
-        <v>1</v>
-      </c>
-      <c r="U35" s="6">
-        <v>0</v>
-      </c>
-      <c r="V35" s="6">
-        <v>0</v>
-      </c>
-      <c r="W35" s="16">
-        <v>0</v>
-      </c>
-      <c r="X35" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y35" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z35" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA35" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>148</v>
-      </c>
-      <c r="AC35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" s="3">
-        <v>0</v>
-      </c>
-      <c r="D36" s="10">
-        <v>11111</v>
-      </c>
-      <c r="E36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x1F</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>17</v>
+      <c r="J36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L36" s="6">
         <v>0</v>
@@ -4129,16 +4155,16 @@
         <v>0</v>
       </c>
       <c r="P36" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q36" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R36" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S36" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T36" s="6">
         <v>1</v>
@@ -4153,40 +4179,40 @@
         <v>0</v>
       </c>
       <c r="X36" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y36" s="22">
-        <v>1100100</v>
+        <v>0</v>
       </c>
       <c r="Z36" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA36" s="23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AB36" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC36" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>10000</v>
+        <v>11111</v>
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x10</v>
+        <v>0x1F</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>17</v>
@@ -4203,8 +4229,8 @@
       <c r="J37" t="s">
         <v>17</v>
       </c>
-      <c r="K37" s="13" t="s">
-        <v>17</v>
+      <c r="K37" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L37" s="6">
         <v>0</v>
@@ -4243,40 +4269,40 @@
         <v>0</v>
       </c>
       <c r="X37" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y37" s="22">
         <v>1100100</v>
       </c>
       <c r="Z37" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA37" s="25" t="s">
-        <v>163</v>
+        <v>73</v>
+      </c>
+      <c r="AA37" s="23" t="s">
+        <v>160</v>
       </c>
       <c r="AB37" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" s="3">
         <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>10001</v>
+        <v>10000</v>
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x11</v>
+        <v>0x10</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>17</v>
@@ -4293,8 +4319,8 @@
       <c r="J38" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="13" t="s">
-        <v>17</v>
+      <c r="K38" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L38" s="6">
         <v>0</v>
@@ -4333,40 +4359,40 @@
         <v>0</v>
       </c>
       <c r="X38" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y38" s="22">
         <v>1100100</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA38" s="25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AB38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
       </c>
       <c r="D39" s="10">
-        <v>10010</v>
+        <v>10001</v>
       </c>
       <c r="E39" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x12</v>
+        <v>0x11</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>17</v>
@@ -4383,8 +4409,8 @@
       <c r="J39" t="s">
         <v>17</v>
       </c>
-      <c r="K39" s="13" t="s">
-        <v>17</v>
+      <c r="K39" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L39" s="6">
         <v>0</v>
@@ -4423,40 +4449,40 @@
         <v>0</v>
       </c>
       <c r="X39" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y39" s="22">
         <v>1100100</v>
       </c>
       <c r="Z39" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA39" s="25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AB39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC39" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
       </c>
       <c r="D40" s="10">
-        <v>10011</v>
+        <v>10010</v>
       </c>
       <c r="E40" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x13</v>
+        <v>0x12</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>17</v>
@@ -4473,8 +4499,8 @@
       <c r="J40" t="s">
         <v>17</v>
       </c>
-      <c r="K40" s="13" t="s">
-        <v>17</v>
+      <c r="K40" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L40" s="6">
         <v>0</v>
@@ -4513,40 +4539,40 @@
         <v>0</v>
       </c>
       <c r="X40" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y40" s="22">
         <v>1100100</v>
       </c>
       <c r="Z40" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA40" s="25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AB40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
       </c>
       <c r="D41" s="10">
-        <v>10100</v>
+        <v>10011</v>
       </c>
       <c r="E41" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x14</v>
+        <v>0x13</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>17</v>
@@ -4563,8 +4589,8 @@
       <c r="J41" t="s">
         <v>17</v>
       </c>
-      <c r="K41" s="13" t="s">
-        <v>17</v>
+      <c r="K41" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L41" s="6">
         <v>0</v>
@@ -4579,19 +4605,19 @@
         <v>0</v>
       </c>
       <c r="P41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U41" s="6">
         <v>0</v>
@@ -4603,40 +4629,40 @@
         <v>0</v>
       </c>
       <c r="X41" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y41" s="22">
         <v>1100100</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AA41" s="23" t="s">
-        <v>167</v>
+        <v>73</v>
+      </c>
+      <c r="AA41" s="25" t="s">
+        <v>164</v>
       </c>
       <c r="AB41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC41" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C42" s="3">
         <v>0</v>
       </c>
       <c r="D42" s="10">
-        <v>10101</v>
+        <v>10100</v>
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x15</v>
+        <v>0x14</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>17</v>
@@ -4653,8 +4679,8 @@
       <c r="J42" t="s">
         <v>17</v>
       </c>
-      <c r="K42" s="13" t="s">
-        <v>17</v>
+      <c r="K42" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L42" s="6">
         <v>0</v>
@@ -4693,22 +4719,22 @@
         <v>0</v>
       </c>
       <c r="X42" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y42" s="22">
         <v>1100100</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AA42" s="23" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="AB42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4716,17 +4742,17 @@
         <v>156</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
       </c>
       <c r="D43" s="10">
-        <v>10110</v>
+        <v>10101</v>
       </c>
       <c r="E43" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x16</v>
+        <v>0x15</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>17</v>
@@ -4743,8 +4769,8 @@
       <c r="J43" t="s">
         <v>17</v>
       </c>
-      <c r="K43" s="13" t="s">
-        <v>17</v>
+      <c r="K43" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L43" s="6">
         <v>0</v>
@@ -4783,40 +4809,40 @@
         <v>0</v>
       </c>
       <c r="X43" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y43" s="22">
         <v>1100100</v>
       </c>
       <c r="Z43" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AA43" s="23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AB43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
       </c>
       <c r="D44" s="10">
-        <v>10111</v>
+        <v>10110</v>
       </c>
       <c r="E44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x17</v>
+        <v>0x16</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>17</v>
@@ -4824,7 +4850,7 @@
       <c r="G44" t="s">
         <v>17</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I44" s="13" t="s">
@@ -4833,8 +4859,8 @@
       <c r="J44" t="s">
         <v>17</v>
       </c>
-      <c r="K44" s="13" t="s">
-        <v>17</v>
+      <c r="K44" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L44" s="6">
         <v>0</v>
@@ -4869,62 +4895,62 @@
       <c r="V44" s="6">
         <v>0</v>
       </c>
-      <c r="W44" s="13">
+      <c r="W44" s="16">
         <v>0</v>
       </c>
       <c r="X44" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y44" s="22">
         <v>1100100</v>
       </c>
       <c r="Z44" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AA44" s="23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AB44" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC44" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>65</v>
+      <c r="A45" s="19" t="s">
+        <v>155</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
       </c>
       <c r="D45" s="10">
-        <v>11010</v>
+        <v>10111</v>
       </c>
       <c r="E45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1A</v>
+        <v>0x17</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" t="s">
         <v>17</v>
       </c>
       <c r="I45" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K45" s="13" t="s">
-        <v>17</v>
+      <c r="J45" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L45" s="6">
         <v>0</v>
@@ -4951,7 +4977,7 @@
         <v>1</v>
       </c>
       <c r="T45" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U45" s="6">
         <v>0</v>
@@ -4963,136 +4989,136 @@
         <v>0</v>
       </c>
       <c r="X45" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y45" s="22">
-        <v>0</v>
+        <v>1100100</v>
       </c>
       <c r="Z45" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA45" s="23">
-        <v>0</v>
+        <v>152</v>
+      </c>
+      <c r="AA45" s="23" t="s">
+        <v>161</v>
       </c>
       <c r="AB45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC45" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46" s="3">
         <v>0</v>
       </c>
       <c r="D46" s="10">
-        <v>11100</v>
+        <v>11010</v>
       </c>
       <c r="E46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1C</v>
+        <v>0x1A</v>
       </c>
       <c r="F46" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K46" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="L46" s="6">
+        <v>0</v>
+      </c>
+      <c r="M46" s="6">
+        <v>0</v>
+      </c>
+      <c r="N46" s="6">
+        <v>0</v>
+      </c>
+      <c r="O46" s="6">
+        <v>0</v>
+      </c>
+      <c r="P46" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="6">
+        <v>1</v>
+      </c>
+      <c r="R46" s="6">
+        <v>1</v>
+      </c>
+      <c r="S46" s="6">
+        <v>1</v>
+      </c>
+      <c r="T46" s="6">
+        <v>1</v>
+      </c>
+      <c r="U46" s="6">
+        <v>0</v>
+      </c>
+      <c r="V46" s="6">
+        <v>0</v>
+      </c>
+      <c r="W46" s="16">
+        <v>0</v>
+      </c>
+      <c r="X46" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y46" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA46" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB46" t="s">
         <v>146</v>
       </c>
-      <c r="G46" t="s">
-        <v>141</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I46" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K46" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L46" s="6">
-        <v>0</v>
-      </c>
-      <c r="M46" s="6">
-        <v>0</v>
-      </c>
-      <c r="N46" s="6">
-        <v>0</v>
-      </c>
-      <c r="O46" s="6">
-        <v>0</v>
-      </c>
-      <c r="P46" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q46" s="6">
-        <v>1</v>
-      </c>
-      <c r="R46" s="6">
-        <v>1</v>
-      </c>
-      <c r="S46" s="6">
-        <v>1</v>
-      </c>
-      <c r="T46" s="6">
-        <v>1</v>
-      </c>
-      <c r="U46" s="6">
-        <v>0</v>
-      </c>
-      <c r="V46" s="6">
-        <v>0</v>
-      </c>
-      <c r="W46" s="16">
-        <v>0</v>
-      </c>
-      <c r="X46" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y46" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA46" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB46" t="s">
-        <v>148</v>
-      </c>
       <c r="AC46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" s="3">
         <v>0</v>
       </c>
       <c r="D47" s="10">
-        <v>11101</v>
+        <v>11100</v>
       </c>
       <c r="E47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1D</v>
+        <v>0x1C</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="G47" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>17</v>
@@ -5103,8 +5129,8 @@
       <c r="J47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K47" s="13" t="s">
-        <v>17</v>
+      <c r="K47" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L47" s="6">
         <v>0</v>
@@ -5143,46 +5169,46 @@
         <v>0</v>
       </c>
       <c r="X47" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y47" s="22">
         <v>0</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA47" s="23">
         <v>0</v>
       </c>
       <c r="AB47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC47" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C48" s="3">
         <v>0</v>
       </c>
       <c r="D48" s="10">
-        <v>111010</v>
+        <v>11101</v>
       </c>
       <c r="E48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3A</v>
+        <v>0x1D</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="G48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>17</v>
@@ -5193,8 +5219,8 @@
       <c r="J48" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K48" s="13" t="s">
-        <v>17</v>
+      <c r="K48" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L48" s="6">
         <v>0</v>
@@ -5209,70 +5235,70 @@
         <v>0</v>
       </c>
       <c r="P48" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q48" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S48" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T48" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U48" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V48" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W48" s="16">
         <v>0</v>
       </c>
       <c r="X48" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y48" s="22">
         <v>0</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA48" s="23">
         <v>0</v>
       </c>
       <c r="AB48" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC48" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C49" s="3">
         <v>0</v>
       </c>
       <c r="D49" s="10">
-        <v>111011</v>
+        <v>111010</v>
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3B</v>
+        <v>0x3A</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>17</v>
@@ -5283,8 +5309,8 @@
       <c r="J49" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K49" s="13" t="s">
-        <v>17</v>
+      <c r="K49" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L49" s="6">
         <v>0</v>
@@ -5323,46 +5349,46 @@
         <v>0</v>
       </c>
       <c r="X49" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y49" s="22">
         <v>0</v>
       </c>
       <c r="Z49" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA49" s="23">
         <v>0</v>
       </c>
       <c r="AB49" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC49" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C50" s="3">
         <v>0</v>
       </c>
       <c r="D50" s="10">
-        <v>111001</v>
+        <v>111011</v>
       </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x39</v>
+        <v>0x3B</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="G50" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>17</v>
@@ -5373,11 +5399,11 @@
       <c r="J50" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K50" s="13" t="s">
-        <v>17</v>
+      <c r="K50" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L50" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M50" s="6">
         <v>0</v>
@@ -5404,49 +5430,49 @@
         <v>0</v>
       </c>
       <c r="U50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W50" s="16">
         <v>0</v>
       </c>
       <c r="X50" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y50" s="22">
         <v>0</v>
       </c>
       <c r="Z50" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA50" s="23">
         <v>0</v>
       </c>
       <c r="AB50" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC50" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C51" s="3">
         <v>0</v>
       </c>
       <c r="D51" s="10">
-        <v>1110000</v>
+        <v>111001</v>
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x70</v>
+        <v>0x39</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>17</v>
@@ -5463,14 +5489,14 @@
       <c r="J51" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K51" s="13" t="s">
-        <v>17</v>
+      <c r="K51" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L51" s="6">
         <v>1</v>
       </c>
       <c r="M51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51" s="6">
         <v>0</v>
@@ -5479,64 +5505,64 @@
         <v>0</v>
       </c>
       <c r="P51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W51" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X51" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y51" s="22">
         <v>0</v>
       </c>
       <c r="Z51" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA51" s="23">
         <v>0</v>
       </c>
       <c r="AB51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC51" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C52" s="3">
         <v>0</v>
       </c>
       <c r="D52" s="10">
-        <v>1110001</v>
+        <v>1110000</v>
       </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x71</v>
+        <v>0x70</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>17</v>
@@ -5553,8 +5579,8 @@
       <c r="J52" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K52" s="13" t="s">
-        <v>17</v>
+      <c r="K52" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L52" s="6">
         <v>1</v>
@@ -5593,40 +5619,40 @@
         <v>1</v>
       </c>
       <c r="X52" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y52" s="22">
         <v>0</v>
       </c>
       <c r="Z52" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA52" s="23">
         <v>0</v>
       </c>
       <c r="AB52" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC52" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C53" s="3">
         <v>0</v>
       </c>
       <c r="D53" s="10">
-        <v>1110010</v>
+        <v>1110001</v>
       </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x72</v>
+        <v>0x71</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>17</v>
@@ -5643,8 +5669,8 @@
       <c r="J53" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K53" s="13" t="s">
-        <v>17</v>
+      <c r="K53" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L53" s="6">
         <v>1</v>
@@ -5683,40 +5709,40 @@
         <v>1</v>
       </c>
       <c r="X53" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y53" s="22">
         <v>0</v>
       </c>
       <c r="Z53" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA53" s="23">
         <v>0</v>
       </c>
       <c r="AB53" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC53" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C54" s="3">
         <v>0</v>
       </c>
       <c r="D54" s="10">
-        <v>1110011</v>
+        <v>1110010</v>
       </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x73</v>
+        <v>0x72</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>17</v>
@@ -5733,8 +5759,8 @@
       <c r="J54" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K54" s="13" t="s">
-        <v>17</v>
+      <c r="K54" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L54" s="6">
         <v>1</v>
@@ -5773,40 +5799,40 @@
         <v>1</v>
       </c>
       <c r="X54" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y54" s="22">
         <v>0</v>
       </c>
       <c r="Z54" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA54" s="23">
         <v>0</v>
       </c>
       <c r="AB54" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC54" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C55" s="3">
         <v>0</v>
       </c>
       <c r="D55" s="10">
-        <v>1110100</v>
+        <v>1110011</v>
       </c>
       <c r="E55" s="3" t="str">
-        <f t="shared" ref="E55:E56" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C55,7) + BIN2DEC($D55)))</f>
-        <v>0x74</v>
+        <f t="shared" si="1"/>
+        <v>0x73</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>17</v>
@@ -5823,8 +5849,8 @@
       <c r="J55" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K55" s="13" t="s">
-        <v>17</v>
+      <c r="K55" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="L55" s="6">
         <v>1</v>
@@ -5863,112 +5889,202 @@
         <v>1</v>
       </c>
       <c r="X55" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y55" s="22">
         <v>0</v>
       </c>
       <c r="Z55" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AA55" s="23">
         <v>0</v>
       </c>
       <c r="AB55" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC55" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="3">
+        <v>0</v>
+      </c>
+      <c r="D56" s="10">
+        <v>1110100</v>
+      </c>
+      <c r="E56" s="3" t="str">
+        <f t="shared" ref="E56:E57" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C56,7) + BIN2DEC($D56)))</f>
+        <v>0x74</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K56" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="L56" s="6">
+        <v>1</v>
+      </c>
+      <c r="M56" s="6">
+        <v>1</v>
+      </c>
+      <c r="N56" s="6">
+        <v>0</v>
+      </c>
+      <c r="O56" s="6">
+        <v>0</v>
+      </c>
+      <c r="P56" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="6">
+        <v>1</v>
+      </c>
+      <c r="R56" s="6">
+        <v>1</v>
+      </c>
+      <c r="S56" s="6">
+        <v>1</v>
+      </c>
+      <c r="T56" s="6">
+        <v>1</v>
+      </c>
+      <c r="U56" s="6">
+        <v>1</v>
+      </c>
+      <c r="V56" s="6">
+        <v>1</v>
+      </c>
+      <c r="W56" s="16">
+        <v>1</v>
+      </c>
+      <c r="X56" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y56" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA56" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="3">
-        <v>0</v>
-      </c>
-      <c r="D56" s="10">
+      <c r="B57" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="3">
+        <v>0</v>
+      </c>
+      <c r="D57" s="10">
         <v>1111000</v>
       </c>
-      <c r="E56" s="3" t="str">
+      <c r="E57" s="3" t="str">
         <f t="shared" si="2"/>
         <v>0x78</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G56" t="s">
-        <v>17</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I56" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K56" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L56" s="6">
-        <v>1</v>
-      </c>
-      <c r="M56" s="6">
-        <v>1</v>
-      </c>
-      <c r="N56" s="6">
-        <v>0</v>
-      </c>
-      <c r="O56" s="6">
-        <v>0</v>
-      </c>
-      <c r="P56" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q56" s="6">
-        <v>1</v>
-      </c>
-      <c r="R56" s="6">
-        <v>1</v>
-      </c>
-      <c r="S56" s="6">
-        <v>1</v>
-      </c>
-      <c r="T56" s="6">
-        <v>1</v>
-      </c>
-      <c r="U56" s="6">
-        <v>1</v>
-      </c>
-      <c r="V56" s="6">
-        <v>1</v>
-      </c>
-      <c r="W56" s="16">
-        <v>1</v>
-      </c>
-      <c r="X56" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y56" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z56" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA56" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB56" t="s">
-        <v>148</v>
-      </c>
-      <c r="AC56" t="s">
-        <v>140</v>
+      <c r="F57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G57" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K57" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="L57" s="6">
+        <v>1</v>
+      </c>
+      <c r="M57" s="6">
+        <v>1</v>
+      </c>
+      <c r="N57" s="6">
+        <v>0</v>
+      </c>
+      <c r="O57" s="6">
+        <v>0</v>
+      </c>
+      <c r="P57" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="6">
+        <v>1</v>
+      </c>
+      <c r="R57" s="6">
+        <v>1</v>
+      </c>
+      <c r="S57" s="6">
+        <v>1</v>
+      </c>
+      <c r="T57" s="6">
+        <v>1</v>
+      </c>
+      <c r="U57" s="6">
+        <v>1</v>
+      </c>
+      <c r="V57" s="6">
+        <v>1</v>
+      </c>
+      <c r="W57" s="16">
+        <v>1</v>
+      </c>
+      <c r="X57" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y57" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA57" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
instruction field is explicitly hex now, no longer binary
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E1A0C5-DA16-A346-823A-DA3C8D4DC6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D2F4FA-9CDB-D743-B6F3-269CD2108FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="178">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>0x022b02fc</t>
+  </si>
+  <si>
+    <t>0x4d</t>
+  </si>
+  <si>
+    <t>0x7d</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1050,10 @@
   <dimension ref="A1:AC57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S40" sqref="S40"/>
+      <selection pane="bottomRight" activeCell="Y60" sqref="Y60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1275,8 +1281,8 @@
       <c r="X3" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y3" s="22">
-        <v>0</v>
+      <c r="Y3" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>73</v>
@@ -1365,8 +1371,8 @@
       <c r="X4" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y4" s="22">
-        <v>0</v>
+      <c r="Y4" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>73</v>
@@ -1455,8 +1461,8 @@
       <c r="X5" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y5" s="22">
-        <v>0</v>
+      <c r="Y5" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>73</v>
@@ -1545,8 +1551,8 @@
       <c r="X6" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y6" s="22">
-        <v>0</v>
+      <c r="Y6" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>73</v>
@@ -1635,8 +1641,8 @@
       <c r="X7" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y7" s="22">
-        <v>0</v>
+      <c r="Y7" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z7" s="3" t="s">
         <v>73</v>
@@ -1725,8 +1731,8 @@
       <c r="X8" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y8" s="22">
-        <v>0</v>
+      <c r="Y8" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z8" s="3" t="s">
         <v>73</v>
@@ -1815,8 +1821,8 @@
       <c r="X9" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y9" s="22">
-        <v>0</v>
+      <c r="Y9" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z9" s="3" t="s">
         <v>73</v>
@@ -1905,8 +1911,8 @@
       <c r="X10" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="Y10" s="22">
-        <v>0</v>
+      <c r="Y10" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z10" s="3" t="s">
         <v>169</v>
@@ -1992,8 +1998,8 @@
       <c r="X11" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y11" s="22">
-        <v>0</v>
+      <c r="Y11" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>73</v>
@@ -2082,8 +2088,8 @@
       <c r="X12" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y12" s="22">
-        <v>1100100</v>
+      <c r="Y12" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>175</v>
@@ -2172,8 +2178,8 @@
       <c r="X13" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y13" s="22">
-        <v>0</v>
+      <c r="Y13" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z13" s="3" t="s">
         <v>73</v>
@@ -2262,8 +2268,8 @@
       <c r="X14" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y14" s="22">
-        <v>0</v>
+      <c r="Y14" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z14" s="3" t="s">
         <v>73</v>
@@ -2352,8 +2358,8 @@
       <c r="X15" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y15" s="22">
-        <v>0</v>
+      <c r="Y15" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z15" s="3" t="s">
         <v>73</v>
@@ -2442,8 +2448,8 @@
       <c r="X16" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y16" s="22">
-        <v>0</v>
+      <c r="Y16" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z16" s="3" t="s">
         <v>73</v>
@@ -2532,8 +2538,8 @@
       <c r="X17" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y17" s="22">
-        <v>0</v>
+      <c r="Y17" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z17" s="3" t="s">
         <v>73</v>
@@ -2622,8 +2628,8 @@
       <c r="X18" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y18" s="22">
-        <v>0</v>
+      <c r="Y18" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z18" s="3" t="s">
         <v>73</v>
@@ -2712,8 +2718,8 @@
       <c r="X19" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y19" s="22">
-        <v>0</v>
+      <c r="Y19" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z19" s="3" t="s">
         <v>73</v>
@@ -2802,8 +2808,8 @@
       <c r="X20" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y20" s="22">
-        <v>0</v>
+      <c r="Y20" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z20" s="3" t="s">
         <v>73</v>
@@ -2892,8 +2898,8 @@
       <c r="X21" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y21" s="22">
-        <v>0</v>
+      <c r="Y21" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z21" s="3" t="s">
         <v>73</v>
@@ -2982,8 +2988,8 @@
       <c r="X22" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y22" s="22">
-        <v>0</v>
+      <c r="Y22" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z22" s="3" t="s">
         <v>73</v>
@@ -3072,8 +3078,8 @@
       <c r="X23" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y23" s="22">
-        <v>0</v>
+      <c r="Y23" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z23" s="3" t="s">
         <v>73</v>
@@ -3162,8 +3168,8 @@
       <c r="X24" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y24" s="22">
-        <v>0</v>
+      <c r="Y24" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="Z24" s="3" t="s">
         <v>73</v>
@@ -3280,8 +3286,8 @@
       <c r="X26" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y26" s="22">
-        <v>0</v>
+      <c r="Y26" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z26" s="3" t="s">
         <v>73</v>
@@ -3370,8 +3376,8 @@
       <c r="X27" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y27" s="22">
-        <v>0</v>
+      <c r="Y27" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z27" s="3" t="s">
         <v>73</v>
@@ -3460,8 +3466,8 @@
       <c r="X28" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y28" s="22">
-        <v>0</v>
+      <c r="Y28" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z28" s="3" t="s">
         <v>73</v>
@@ -3550,8 +3556,8 @@
       <c r="X29" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y29" s="22">
-        <v>0</v>
+      <c r="Y29" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z29" s="3" t="s">
         <v>73</v>
@@ -3640,8 +3646,8 @@
       <c r="X30" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y30" s="22">
-        <v>0</v>
+      <c r="Y30" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z30" s="3" t="s">
         <v>73</v>
@@ -3730,8 +3736,8 @@
       <c r="X31" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y31" s="22">
-        <v>0</v>
+      <c r="Y31" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z31" s="3" t="s">
         <v>73</v>
@@ -3820,8 +3826,8 @@
       <c r="X32" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y32" s="22">
-        <v>0</v>
+      <c r="Y32" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z32" s="3" t="s">
         <v>73</v>
@@ -3910,8 +3916,8 @@
       <c r="X33" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y33" s="22">
-        <v>0</v>
+      <c r="Y33" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z33" s="3" t="s">
         <v>73</v>
@@ -4000,8 +4006,8 @@
       <c r="X34" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y34" s="22">
-        <v>0</v>
+      <c r="Y34" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z34" s="3" t="s">
         <v>73</v>
@@ -4090,8 +4096,8 @@
       <c r="X35" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y35" s="22">
-        <v>0</v>
+      <c r="Y35" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z35" s="3" t="s">
         <v>73</v>
@@ -4181,8 +4187,8 @@
       <c r="X36" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y36" s="22">
-        <v>0</v>
+      <c r="Y36" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z36" s="3" t="s">
         <v>73</v>
@@ -4271,8 +4277,8 @@
       <c r="X37" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y37" s="22">
-        <v>1100100</v>
+      <c r="Y37" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z37" s="3" t="s">
         <v>73</v>
@@ -4361,8 +4367,8 @@
       <c r="X38" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y38" s="22">
-        <v>1100100</v>
+      <c r="Y38" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z38" s="3" t="s">
         <v>73</v>
@@ -4451,8 +4457,8 @@
       <c r="X39" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y39" s="22">
-        <v>1100100</v>
+      <c r="Y39" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z39" s="3" t="s">
         <v>73</v>
@@ -4541,8 +4547,8 @@
       <c r="X40" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y40" s="22">
-        <v>1100100</v>
+      <c r="Y40" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z40" s="3" t="s">
         <v>73</v>
@@ -4631,8 +4637,8 @@
       <c r="X41" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y41" s="22">
-        <v>1100100</v>
+      <c r="Y41" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z41" s="3" t="s">
         <v>73</v>
@@ -4721,8 +4727,8 @@
       <c r="X42" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y42" s="22">
-        <v>1100100</v>
+      <c r="Y42" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z42" s="3" t="s">
         <v>152</v>
@@ -4811,8 +4817,8 @@
       <c r="X43" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y43" s="22">
-        <v>1100100</v>
+      <c r="Y43" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z43" s="3" t="s">
         <v>152</v>
@@ -4901,8 +4907,8 @@
       <c r="X44" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y44" s="22">
-        <v>1100100</v>
+      <c r="Y44" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z44" s="3" t="s">
         <v>152</v>
@@ -4991,8 +4997,8 @@
       <c r="X45" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y45" s="22">
-        <v>1100100</v>
+      <c r="Y45" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z45" s="3" t="s">
         <v>152</v>
@@ -5081,8 +5087,8 @@
       <c r="X46" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y46" s="22">
-        <v>0</v>
+      <c r="Y46" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z46" s="3" t="s">
         <v>73</v>
@@ -5171,8 +5177,8 @@
       <c r="X47" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y47" s="22">
-        <v>0</v>
+      <c r="Y47" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z47" s="3" t="s">
         <v>73</v>
@@ -5261,8 +5267,8 @@
       <c r="X48" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y48" s="22">
-        <v>0</v>
+      <c r="Y48" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z48" s="3" t="s">
         <v>73</v>
@@ -5351,8 +5357,8 @@
       <c r="X49" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y49" s="22">
-        <v>0</v>
+      <c r="Y49" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z49" s="3" t="s">
         <v>73</v>
@@ -5441,8 +5447,8 @@
       <c r="X50" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y50" s="22">
-        <v>0</v>
+      <c r="Y50" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z50" s="3" t="s">
         <v>73</v>
@@ -5531,8 +5537,8 @@
       <c r="X51" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y51" s="22">
-        <v>0</v>
+      <c r="Y51" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z51" s="3" t="s">
         <v>73</v>
@@ -5621,8 +5627,8 @@
       <c r="X52" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y52" s="22">
-        <v>0</v>
+      <c r="Y52" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z52" s="3" t="s">
         <v>73</v>
@@ -5711,8 +5717,8 @@
       <c r="X53" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y53" s="22">
-        <v>0</v>
+      <c r="Y53" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z53" s="3" t="s">
         <v>73</v>
@@ -5801,8 +5807,8 @@
       <c r="X54" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y54" s="22">
-        <v>0</v>
+      <c r="Y54" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z54" s="3" t="s">
         <v>73</v>
@@ -5891,8 +5897,8 @@
       <c r="X55" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y55" s="22">
-        <v>0</v>
+      <c r="Y55" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z55" s="3" t="s">
         <v>73</v>
@@ -5981,8 +5987,8 @@
       <c r="X56" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y56" s="22">
-        <v>0</v>
+      <c r="Y56" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z56" s="3" t="s">
         <v>73</v>
@@ -6071,8 +6077,8 @@
       <c r="X57" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Y57" s="22">
-        <v>0</v>
+      <c r="Y57" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="Z57" s="3" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
cmos command addresses are ZERO OFFSET
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF93DCD4-66E2-C147-AFCB-A48CAE860C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B469329-DB3C-7E46-B9EA-FCF99080883B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -477,45 +477,18 @@
     <t>read_ring_pc_wr_ptr</t>
   </si>
   <si>
-    <t>0x38000248</t>
-  </si>
-  <si>
-    <t>0x38000244</t>
-  </si>
-  <si>
     <t>read_cmos_fpga_temp</t>
   </si>
   <si>
     <t>read_cmos_sensor_temp</t>
   </si>
   <si>
-    <t>0x380001f0</t>
-  </si>
-  <si>
-    <t>0x380001f4</t>
-  </si>
-  <si>
     <t>noop</t>
   </si>
   <si>
     <t>start_cmos_init</t>
   </si>
   <si>
-    <t>0x38000040</t>
-  </si>
-  <si>
-    <t>0x38000044</t>
-  </si>
-  <si>
-    <t>0x38000048</t>
-  </si>
-  <si>
-    <t>0x38000050</t>
-  </si>
-  <si>
-    <t>0x38000054</t>
-  </si>
-  <si>
     <t>0xf0851001</t>
   </si>
   <si>
@@ -567,10 +540,37 @@
     <t>linetime</t>
   </si>
   <si>
-    <t>0x38000100</t>
-  </si>
-  <si>
     <t>check line time for last init command</t>
+  </si>
+  <si>
+    <t>0x00000244</t>
+  </si>
+  <si>
+    <t>0x00000248</t>
+  </si>
+  <si>
+    <t>0x000001f4</t>
+  </si>
+  <si>
+    <t>0x000001f0</t>
+  </si>
+  <si>
+    <t>0x0000100</t>
+  </si>
+  <si>
+    <t>0x00000040</t>
+  </si>
+  <si>
+    <t>0x00000044</t>
+  </si>
+  <si>
+    <t>0x00000048</t>
+  </si>
+  <si>
+    <t>0x00000050</t>
+  </si>
+  <si>
+    <t>0x00000054</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1048,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z18" sqref="Z18"/>
+      <selection pane="bottomRight" activeCell="Z35" sqref="Z35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1910,7 +1910,7 @@
         <v>143</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="AA10" s="25" t="s">
         <v>67</v>
@@ -1919,7 +1919,7 @@
         <v>131</v>
       </c>
       <c r="AC10" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -2000,7 +2000,7 @@
         <v>143</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="AA11" s="23" t="s">
         <v>67</v>
@@ -2009,7 +2009,7 @@
         <v>131</v>
       </c>
       <c r="AC11" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -2099,12 +2099,12 @@
         <v>131</v>
       </c>
       <c r="AC12" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>86</v>
@@ -2180,7 +2180,7 @@
         <v>143</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="AA13" s="23" t="s">
         <v>67</v>
@@ -2189,12 +2189,12 @@
         <v>131</v>
       </c>
       <c r="AC13" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>86</v>
@@ -2270,7 +2270,7 @@
         <v>143</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="AA14" s="23" t="s">
         <v>67</v>
@@ -2279,12 +2279,12 @@
         <v>131</v>
       </c>
       <c r="AC14" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>86</v>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="18" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>86</v>
@@ -2582,7 +2582,7 @@
         <v>17</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="K18" s="23" t="s">
         <v>141</v>
@@ -2630,7 +2630,7 @@
         <v>143</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AA18" s="23" t="s">
         <v>67</v>
@@ -2639,7 +2639,7 @@
         <v>131</v>
       </c>
       <c r="AC18" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4202,7 +4202,7 @@
     </row>
     <row r="37" spans="1:29" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>86</v>
@@ -4278,21 +4278,21 @@
         <v>144</v>
       </c>
       <c r="Z37" s="3" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="AA37" s="23" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="AB37" t="s">
         <v>131</v>
       </c>
       <c r="AC37" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>86</v>
@@ -4368,21 +4368,21 @@
         <v>144</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="AA38" s="23" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="AB38" t="s">
         <v>131</v>
       </c>
       <c r="AC38" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>86</v>
@@ -4458,21 +4458,21 @@
         <v>144</v>
       </c>
       <c r="Z39" s="3" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="AA39" s="23" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="AB39" t="s">
         <v>131</v>
       </c>
       <c r="AC39" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>86</v>
@@ -4557,12 +4557,12 @@
         <v>131</v>
       </c>
       <c r="AC40" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>86</v>
@@ -4638,21 +4638,21 @@
         <v>144</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="AA41" s="23" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="AB41" t="s">
         <v>131</v>
       </c>
       <c r="AC41" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>86</v>
@@ -4728,16 +4728,16 @@
         <v>144</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="AA42" s="23" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="AB42" t="s">
         <v>131</v>
       </c>
       <c r="AC42" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
now believe cmos write value is big endian
</commit_message>
<xml_diff>
--- a/command_deck.xlsx
+++ b/command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B469329-DB3C-7E46-B9EA-FCF99080883B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B70C4B7-F56E-A044-921D-719ED190CCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -489,9 +489,6 @@
     <t>start_cmos_init</t>
   </si>
   <si>
-    <t>0xf0851001</t>
-  </si>
-  <si>
     <t>start CMOS initialization</t>
   </si>
   <si>
@@ -571,6 +568,9 @@
   </si>
   <si>
     <t>0x00000054</t>
+  </si>
+  <si>
+    <t>0x011085f0</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1045,10 @@
   <dimension ref="A1:AC58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="N29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z35" sqref="Z35"/>
+      <selection pane="bottomRight" activeCell="AA42" sqref="AA42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1910,7 +1910,7 @@
         <v>143</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AA10" s="25" t="s">
         <v>67</v>
@@ -1919,7 +1919,7 @@
         <v>131</v>
       </c>
       <c r="AC10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -2000,7 +2000,7 @@
         <v>143</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AA11" s="23" t="s">
         <v>67</v>
@@ -2009,7 +2009,7 @@
         <v>131</v>
       </c>
       <c r="AC11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -2099,7 +2099,7 @@
         <v>131</v>
       </c>
       <c r="AC12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -2180,7 +2180,7 @@
         <v>143</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AA13" s="23" t="s">
         <v>67</v>
@@ -2189,7 +2189,7 @@
         <v>131</v>
       </c>
       <c r="AC13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -2270,7 +2270,7 @@
         <v>143</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AA14" s="23" t="s">
         <v>67</v>
@@ -2279,12 +2279,12 @@
         <v>131</v>
       </c>
       <c r="AC14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>86</v>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="18" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>86</v>
@@ -2582,7 +2582,7 @@
         <v>17</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K18" s="23" t="s">
         <v>141</v>
@@ -2630,7 +2630,7 @@
         <v>143</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AA18" s="23" t="s">
         <v>67</v>
@@ -2639,7 +2639,7 @@
         <v>131</v>
       </c>
       <c r="AC18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4278,21 +4278,21 @@
         <v>144</v>
       </c>
       <c r="Z37" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AA37" s="23" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="AB37" t="s">
         <v>131</v>
       </c>
       <c r="AC37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>86</v>
@@ -4368,21 +4368,21 @@
         <v>144</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AA38" s="23" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="AB38" t="s">
         <v>131</v>
       </c>
       <c r="AC38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>86</v>
@@ -4458,16 +4458,16 @@
         <v>144</v>
       </c>
       <c r="Z39" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AA39" s="23" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="AB39" t="s">
         <v>131</v>
       </c>
       <c r="AC39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -4557,12 +4557,12 @@
         <v>131</v>
       </c>
       <c r="AC40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>86</v>
@@ -4638,21 +4638,21 @@
         <v>144</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AA41" s="23" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="AB41" t="s">
         <v>131</v>
       </c>
       <c r="AC41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>86</v>
@@ -4728,16 +4728,16 @@
         <v>144</v>
       </c>
       <c r="Z42" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA42" s="23" t="s">
         <v>178</v>
-      </c>
-      <c r="AA42" s="23" t="s">
-        <v>151</v>
       </c>
       <c r="AB42" t="s">
         <v>131</v>
       </c>
       <c r="AC42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="16" x14ac:dyDescent="0.2">

</xml_diff>